<commit_message>
Sky News Arabia ShieldW Halted
Sky News Arabia ShieldW Halted
</commit_message>
<xml_diff>
--- a/System_2.1.2.xlsx
+++ b/System_2.1.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F2EFB7-FEF9-49EC-A3B0-7594AC9FB08B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E2582D2-4BB5-431F-83EB-6D7F31BB1A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="585">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="585">
   <si>
     <t>Zone</t>
   </si>
@@ -4724,6 +4724,168 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="74" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4748,12 +4910,6 @@
     <xf numFmtId="0" fontId="39" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
@@ -4775,161 +4931,38 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="74" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="27" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4973,39 +5006,6 @@
     <xf numFmtId="0" fontId="3" fillId="40" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5024,25 +5024,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5120,46 +5141,25 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -6311,7 +6311,7 @@
   <dimension ref="A1:W29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E10" workbookViewId="0">
-      <selection activeCell="V23" sqref="V23"/>
+      <selection activeCell="V20" sqref="V20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6575,7 +6575,7 @@
       <c r="D10" s="108"/>
       <c r="E10" s="68">
         <f>Boat!S8</f>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G10" s="525"/>
       <c r="I10" s="542"/>
@@ -6708,7 +6708,9 @@
       <c r="V13" s="19">
         <v>1</v>
       </c>
-      <c r="W13" s="6"/>
+      <c r="W13" s="6" t="s">
+        <v>580</v>
+      </c>
     </row>
     <row r="14" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="244" t="s">
@@ -6732,15 +6734,9 @@
         <v>220</v>
       </c>
       <c r="I14" s="542"/>
-      <c r="U14" s="6" t="s">
-        <v>580</v>
-      </c>
-      <c r="V14" s="6">
-        <v>1</v>
-      </c>
-      <c r="W14" s="6" t="s">
-        <v>580</v>
-      </c>
+      <c r="U14" s="6"/>
+      <c r="V14" s="6"/>
+      <c r="W14" s="6"/>
     </row>
     <row r="15" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="248" t="s">
@@ -6987,13 +6983,13 @@
       </c>
       <c r="P26" s="444"/>
       <c r="Q26" s="451">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="T26" s="455" t="s">
         <v>542</v>
       </c>
       <c r="V26">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W26" s="19" t="s">
         <v>543</v>
@@ -7229,7 +7225,7 @@
         <v>517</v>
       </c>
       <c r="AM1" s="458"/>
-      <c r="AN1" s="590"/>
+      <c r="AN1" s="587"/>
       <c r="AO1" s="375" t="s">
         <v>487</v>
       </c>
@@ -7238,23 +7234,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="614">
+      <c r="A2" s="569">
         <f ca="1">TODAY()</f>
         <v>45275</v>
       </c>
-      <c r="B2" s="616" t="s">
+      <c r="B2" s="571" t="s">
         <v>379</v>
       </c>
       <c r="C2" s="561" t="s">
         <v>365</v>
       </c>
-      <c r="D2" s="618" t="s">
+      <c r="D2" s="573" t="s">
         <v>362</v>
       </c>
-      <c r="E2" s="563" t="s">
+      <c r="E2" s="617" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="571" t="s">
+      <c r="F2" s="592" t="s">
         <v>103</v>
       </c>
       <c r="G2" s="446" t="s">
@@ -7267,17 +7263,17 @@
       <c r="J2" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="K2" s="565" t="s">
+      <c r="K2" s="619" t="s">
         <v>349</v>
       </c>
-      <c r="L2" s="566"/>
-      <c r="M2" s="571" t="s">
+      <c r="L2" s="620"/>
+      <c r="M2" s="592" t="s">
         <v>103</v>
       </c>
       <c r="N2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="597" t="s">
+      <c r="O2" s="596" t="s">
         <v>103</v>
       </c>
       <c r="P2" s="85" t="s">
@@ -7287,7 +7283,7 @@
         <v>144</v>
       </c>
       <c r="R2" s="524"/>
-      <c r="S2" s="584" t="s">
+      <c r="S2" s="609" t="s">
         <v>149</v>
       </c>
       <c r="T2" s="89"/>
@@ -7320,15 +7316,15 @@
         <v>481</v>
       </c>
       <c r="AM2" s="485"/>
-      <c r="AN2" s="591"/>
+      <c r="AN2" s="588"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="615"/>
-      <c r="B3" s="617"/>
+      <c r="A3" s="570"/>
+      <c r="B3" s="572"/>
       <c r="C3" s="562"/>
-      <c r="D3" s="619"/>
-      <c r="E3" s="564"/>
-      <c r="F3" s="572"/>
+      <c r="D3" s="574"/>
+      <c r="E3" s="618"/>
+      <c r="F3" s="593"/>
       <c r="G3" s="447" t="s">
         <v>28</v>
       </c>
@@ -7347,17 +7343,17 @@
       <c r="L3" s="211" t="s">
         <v>108</v>
       </c>
-      <c r="M3" s="572"/>
+      <c r="M3" s="593"/>
       <c r="N3" s="69" t="s">
         <v>147</v>
       </c>
-      <c r="O3" s="598"/>
+      <c r="O3" s="597"/>
       <c r="P3" s="2" t="s">
         <v>155</v>
       </c>
       <c r="Q3" s="562"/>
       <c r="R3" s="526"/>
-      <c r="S3" s="586"/>
+      <c r="S3" s="610"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -7374,7 +7370,7 @@
       <c r="AC3" s="100" t="s">
         <v>498</v>
       </c>
-      <c r="AD3" s="581" t="s">
+      <c r="AD3" s="608" t="s">
         <v>473</v>
       </c>
       <c r="AE3" s="272"/>
@@ -7386,13 +7382,13 @@
       <c r="AK3" s="272"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="485"/>
-      <c r="AN3" s="591"/>
+      <c r="AN3" s="588"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="251" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="630" t="s">
+      <c r="B4" s="585" t="s">
         <v>382</v>
       </c>
       <c r="C4" s="561" t="s">
@@ -7404,7 +7400,7 @@
       <c r="E4" s="422">
         <v>1</v>
       </c>
-      <c r="F4" s="572"/>
+      <c r="F4" s="593"/>
       <c r="G4" s="427" t="s">
         <v>203</v>
       </c>
@@ -7421,11 +7417,11 @@
         <v>151</v>
       </c>
       <c r="L4" s="214"/>
-      <c r="M4" s="572"/>
+      <c r="M4" s="593"/>
       <c r="N4" s="179" t="s">
         <v>70</v>
       </c>
-      <c r="O4" s="598"/>
+      <c r="O4" s="597"/>
       <c r="P4" s="2" t="s">
         <v>192</v>
       </c>
@@ -7452,7 +7448,7 @@
       <c r="AA4" s="325"/>
       <c r="AB4" s="219"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="581"/>
+      <c r="AD4" s="608"/>
       <c r="AE4" s="272"/>
       <c r="AF4" s="272"/>
       <c r="AG4" s="16"/>
@@ -7462,7 +7458,7 @@
       <c r="AK4" s="272"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="485"/>
-      <c r="AN4" s="591"/>
+      <c r="AN4" s="588"/>
       <c r="AO4" s="375" t="s">
         <v>91</v>
       </c>
@@ -7471,7 +7467,7 @@
       <c r="A5" s="559" t="s">
         <v>435</v>
       </c>
-      <c r="B5" s="631"/>
+      <c r="B5" s="586"/>
       <c r="C5" s="562"/>
       <c r="D5" s="61" t="s">
         <v>154</v>
@@ -7479,20 +7475,20 @@
       <c r="E5" s="423">
         <v>1</v>
       </c>
-      <c r="F5" s="572"/>
-      <c r="G5" s="622" t="s">
+      <c r="F5" s="593"/>
+      <c r="G5" s="577" t="s">
         <v>193</v>
       </c>
-      <c r="H5" s="622"/>
-      <c r="I5" s="622"/>
-      <c r="J5" s="622"/>
-      <c r="K5" s="622"/>
-      <c r="L5" s="623"/>
-      <c r="M5" s="572"/>
+      <c r="H5" s="577"/>
+      <c r="I5" s="577"/>
+      <c r="J5" s="577"/>
+      <c r="K5" s="577"/>
+      <c r="L5" s="578"/>
+      <c r="M5" s="593"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
-      <c r="O5" s="598"/>
+      <c r="O5" s="597"/>
       <c r="T5" s="89"/>
       <c r="U5" s="124"/>
       <c r="V5" s="120"/>
@@ -7523,24 +7519,24 @@
       <c r="AK5" s="272"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="485"/>
-      <c r="AN5" s="591"/>
+      <c r="AN5" s="588"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="560"/>
-      <c r="B6" s="628" t="s">
+      <c r="B6" s="583" t="s">
         <v>178</v>
       </c>
       <c r="C6" s="557"/>
       <c r="D6" s="558"/>
-      <c r="F6" s="572"/>
-      <c r="G6" s="624"/>
-      <c r="H6" s="624"/>
-      <c r="I6" s="624"/>
-      <c r="J6" s="624"/>
-      <c r="K6" s="624"/>
-      <c r="L6" s="625"/>
-      <c r="M6" s="572"/>
-      <c r="O6" s="598"/>
+      <c r="F6" s="593"/>
+      <c r="G6" s="579"/>
+      <c r="H6" s="579"/>
+      <c r="I6" s="579"/>
+      <c r="J6" s="579"/>
+      <c r="K6" s="579"/>
+      <c r="L6" s="580"/>
+      <c r="M6" s="593"/>
+      <c r="O6" s="597"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
       <c r="V6" s="98" t="s">
@@ -7564,16 +7560,16 @@
       <c r="AF6" s="272"/>
       <c r="AG6" s="272"/>
       <c r="AH6" s="272"/>
-      <c r="AI6" s="580"/>
+      <c r="AI6" s="602"/>
       <c r="AJ6" s="498" t="s">
         <v>476</v>
       </c>
-      <c r="AK6" s="580" t="s">
+      <c r="AK6" s="602" t="s">
         <v>256</v>
       </c>
       <c r="AL6" s="272"/>
       <c r="AM6" s="485"/>
-      <c r="AN6" s="591"/>
+      <c r="AN6" s="588"/>
       <c r="AO6" s="375" t="s">
         <v>488</v>
       </c>
@@ -7582,7 +7578,7 @@
       <c r="A7" s="245" t="s">
         <v>554</v>
       </c>
-      <c r="B7" s="629"/>
+      <c r="B7" s="584"/>
       <c r="C7" s="212" t="s">
         <v>383</v>
       </c>
@@ -7592,7 +7588,7 @@
       <c r="E7" s="281">
         <v>3</v>
       </c>
-      <c r="F7" s="572"/>
+      <c r="F7" s="593"/>
       <c r="G7" s="448">
         <v>0</v>
       </c>
@@ -7611,8 +7607,8 @@
       <c r="L7" s="222">
         <v>0</v>
       </c>
-      <c r="M7" s="572"/>
-      <c r="O7" s="598"/>
+      <c r="M7" s="593"/>
+      <c r="O7" s="597"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
       </c>
@@ -7636,18 +7632,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="272"/>
       <c r="AF7" s="272"/>
-      <c r="AG7" s="581" t="s">
+      <c r="AG7" s="608" t="s">
         <v>472</v>
       </c>
       <c r="AH7" s="272"/>
-      <c r="AI7" s="580"/>
+      <c r="AI7" s="602"/>
       <c r="AJ7" s="272"/>
-      <c r="AK7" s="580"/>
+      <c r="AK7" s="602"/>
       <c r="AL7" s="80" t="s">
         <v>515</v>
       </c>
       <c r="AM7" s="485"/>
-      <c r="AN7" s="591"/>
+      <c r="AN7" s="588"/>
       <c r="AP7" s="76" t="s">
         <v>489</v>
       </c>
@@ -7664,25 +7660,25 @@
         <f>SUM(G7:N9)</f>
         <v>16</v>
       </c>
-      <c r="F8" s="572"/>
-      <c r="G8" s="623">
-        <v>0</v>
-      </c>
-      <c r="H8" s="620" t="s">
+      <c r="F8" s="593"/>
+      <c r="G8" s="578">
+        <v>0</v>
+      </c>
+      <c r="H8" s="575" t="s">
         <v>105</v>
       </c>
       <c r="I8" s="524"/>
-      <c r="J8" s="620" t="s">
+      <c r="J8" s="575" t="s">
         <v>105</v>
       </c>
-      <c r="K8" s="626"/>
-      <c r="L8" s="582"/>
-      <c r="M8" s="595"/>
-      <c r="N8" s="587">
+      <c r="K8" s="581"/>
+      <c r="L8" s="611"/>
+      <c r="M8" s="594"/>
+      <c r="N8" s="614">
         <f>N5+N11</f>
         <v>15</v>
       </c>
-      <c r="O8" s="598"/>
+      <c r="O8" s="597"/>
       <c r="T8" s="103" t="s">
         <v>44</v>
       </c>
@@ -7700,14 +7696,14 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="272"/>
       <c r="AF8" s="272"/>
-      <c r="AG8" s="581"/>
+      <c r="AG8" s="608"/>
       <c r="AH8" s="272"/>
-      <c r="AI8" s="580"/>
+      <c r="AI8" s="602"/>
       <c r="AJ8" s="272"/>
       <c r="AK8" s="272"/>
       <c r="AL8" s="272"/>
       <c r="AM8" s="485"/>
-      <c r="AN8" s="591"/>
+      <c r="AN8" s="588"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="245" t="s">
@@ -7722,17 +7718,17 @@
       <c r="D9" s="385" t="s">
         <v>286</v>
       </c>
-      <c r="F9" s="572"/>
-      <c r="G9" s="625"/>
-      <c r="H9" s="621"/>
+      <c r="F9" s="593"/>
+      <c r="G9" s="580"/>
+      <c r="H9" s="576"/>
       <c r="I9" s="526"/>
-      <c r="J9" s="621"/>
-      <c r="K9" s="627"/>
-      <c r="L9" s="583"/>
-      <c r="M9" s="596"/>
-      <c r="N9" s="588"/>
-      <c r="O9" s="599"/>
-      <c r="S9" s="584" t="s">
+      <c r="J9" s="576"/>
+      <c r="K9" s="582"/>
+      <c r="L9" s="612"/>
+      <c r="M9" s="595"/>
+      <c r="N9" s="615"/>
+      <c r="O9" s="598"/>
+      <c r="S9" s="609" t="s">
         <v>62</v>
       </c>
       <c r="T9" s="89"/>
@@ -7754,16 +7750,16 @@
       </c>
       <c r="AE9" s="272"/>
       <c r="AF9" s="272"/>
-      <c r="AG9" s="581"/>
+      <c r="AG9" s="608"/>
       <c r="AH9" s="272"/>
-      <c r="AI9" s="580"/>
+      <c r="AI9" s="602"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="580" t="s">
+      <c r="AK9" s="602" t="s">
         <v>256</v>
       </c>
       <c r="AL9" s="272"/>
       <c r="AM9" s="485"/>
-      <c r="AN9" s="591"/>
+      <c r="AN9" s="588"/>
       <c r="AP9" s="2" t="s">
         <v>527</v>
       </c>
@@ -7778,22 +7774,22 @@
       <c r="D10" s="142"/>
       <c r="E10" s="250">
         <f>Boat!S8</f>
-        <v>42</v>
-      </c>
-      <c r="F10" s="572"/>
+        <v>43</v>
+      </c>
+      <c r="F10" s="593"/>
       <c r="N10" s="475" t="s">
         <v>407</v>
       </c>
-      <c r="O10" s="574" t="s">
+      <c r="O10" s="626" t="s">
         <v>103</v>
       </c>
-      <c r="P10" s="600" t="s">
+      <c r="P10" s="599" t="s">
         <v>411</v>
       </c>
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="585"/>
+      <c r="S10" s="613"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>177</v>
@@ -7823,16 +7819,16 @@
       <c r="AF10" s="251" t="s">
         <v>318</v>
       </c>
-      <c r="AG10" s="581"/>
+      <c r="AG10" s="608"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="580"/>
+      <c r="AI10" s="602"/>
       <c r="AJ10" s="272"/>
-      <c r="AK10" s="580"/>
+      <c r="AK10" s="602"/>
       <c r="AL10" s="272"/>
       <c r="AM10" s="499" t="s">
         <v>325</v>
       </c>
-      <c r="AN10" s="591"/>
+      <c r="AN10" s="588"/>
       <c r="AO10" s="214" t="s">
         <v>95</v>
       </c>
@@ -7850,18 +7846,18 @@
       <c r="D11" s="175" t="s">
         <v>362</v>
       </c>
-      <c r="F11" s="572"/>
+      <c r="F11" s="593"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="575"/>
-      <c r="P11" s="601"/>
+      <c r="O11" s="627"/>
+      <c r="P11" s="600"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>222</v>
       </c>
-      <c r="S11" s="585"/>
+      <c r="S11" s="613"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -7885,14 +7881,14 @@
       <c r="AF11" s="272" t="s">
         <v>494</v>
       </c>
-      <c r="AG11" s="581"/>
+      <c r="AG11" s="608"/>
       <c r="AH11" s="272"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="272"/>
       <c r="AK11" s="272"/>
       <c r="AL11" s="272"/>
       <c r="AM11" s="485"/>
-      <c r="AN11" s="591"/>
+      <c r="AN11" s="588"/>
       <c r="AP11" s="76" t="s">
         <v>502</v>
       </c>
@@ -7911,7 +7907,7 @@
       <c r="E12" s="237">
         <v>3</v>
       </c>
-      <c r="F12" s="572"/>
+      <c r="F12" s="593"/>
       <c r="G12" s="374" t="s">
         <v>411</v>
       </c>
@@ -7920,16 +7916,16 @@
       </c>
       <c r="I12" s="530"/>
       <c r="J12" s="530"/>
-      <c r="K12" s="579"/>
+      <c r="K12" s="631"/>
       <c r="L12" s="213"/>
       <c r="M12" s="213"/>
       <c r="N12" s="213"/>
-      <c r="O12" s="575"/>
-      <c r="P12" s="601"/>
+      <c r="O12" s="627"/>
+      <c r="P12" s="600"/>
       <c r="R12" s="122" t="s">
         <v>181</v>
       </c>
-      <c r="S12" s="586"/>
+      <c r="S12" s="610"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -7950,16 +7946,16 @@
       <c r="AC12" s="100" t="s">
         <v>499</v>
       </c>
-      <c r="AD12" s="589" t="s">
+      <c r="AD12" s="616" t="s">
         <v>245</v>
       </c>
       <c r="AE12" s="498" t="s">
         <v>244</v>
       </c>
-      <c r="AF12" s="581" t="s">
+      <c r="AF12" s="608" t="s">
         <v>231</v>
       </c>
-      <c r="AG12" s="581"/>
+      <c r="AG12" s="608"/>
       <c r="AH12" s="251" t="s">
         <v>264</v>
       </c>
@@ -7972,7 +7968,7 @@
       <c r="AM12" s="603" t="s">
         <v>254</v>
       </c>
-      <c r="AN12" s="591"/>
+      <c r="AN12" s="588"/>
       <c r="AO12" s="375" t="s">
         <v>97</v>
       </c>
@@ -7984,17 +7980,17 @@
       <c r="E13" s="505">
         <v>-3</v>
       </c>
-      <c r="F13" s="572"/>
+      <c r="F13" s="593"/>
       <c r="G13" s="530" t="s">
         <v>448</v>
       </c>
       <c r="H13" s="530"/>
       <c r="I13" s="530"/>
-      <c r="J13" s="579"/>
+      <c r="J13" s="631"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="575"/>
-      <c r="P13" s="602"/>
+      <c r="O13" s="627"/>
+      <c r="P13" s="601"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
       </c>
@@ -8015,8 +8011,8 @@
         <v>519</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="589"/>
-      <c r="AF13" s="581"/>
+      <c r="AD13" s="616"/>
+      <c r="AF13" s="608"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="251" t="s">
         <v>314</v>
@@ -8028,7 +8024,7 @@
       <c r="AK13" s="272"/>
       <c r="AL13" s="272"/>
       <c r="AM13" s="603"/>
-      <c r="AN13" s="591"/>
+      <c r="AN13" s="588"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="507"/>
@@ -8036,18 +8032,18 @@
       <c r="C14" s="516"/>
       <c r="D14" s="509"/>
       <c r="E14" s="510"/>
-      <c r="F14" s="572"/>
+      <c r="F14" s="593"/>
       <c r="G14" s="530" t="s">
         <v>447</v>
       </c>
       <c r="H14" s="530"/>
       <c r="I14" s="530"/>
-      <c r="J14" s="579"/>
+      <c r="J14" s="631"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="575"/>
+      <c r="O14" s="627"/>
       <c r="Q14" s="61" t="s">
         <v>562</v>
       </c>
@@ -8068,9 +8064,9 @@
       <c r="AA14" s="325"/>
       <c r="AB14" s="219"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="589"/>
+      <c r="AD14" s="616"/>
       <c r="AE14" s="272"/>
-      <c r="AF14" s="581"/>
+      <c r="AF14" s="608"/>
       <c r="AG14" s="272"/>
       <c r="AH14" s="272"/>
       <c r="AI14" s="70"/>
@@ -8078,7 +8074,7 @@
       <c r="AK14" s="272"/>
       <c r="AL14" s="272"/>
       <c r="AM14" s="603"/>
-      <c r="AN14" s="591"/>
+      <c r="AN14" s="588"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="506" t="s">
@@ -8087,8 +8083,8 @@
       <c r="C15" s="524" t="s">
         <v>382</v>
       </c>
-      <c r="F15" s="572"/>
-      <c r="O15" s="575"/>
+      <c r="F15" s="593"/>
+      <c r="O15" s="627"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -8110,8 +8106,8 @@
       <c r="AC15" s="76" t="s">
         <v>497</v>
       </c>
-      <c r="AD15" s="589"/>
-      <c r="AF15" s="581"/>
+      <c r="AD15" s="616"/>
+      <c r="AF15" s="608"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="251" t="s">
         <v>466</v>
@@ -8125,7 +8121,7 @@
       <c r="AK15" s="272"/>
       <c r="AL15" s="272"/>
       <c r="AM15" s="603"/>
-      <c r="AN15" s="591"/>
+      <c r="AN15" s="588"/>
       <c r="AP15" s="76" t="s">
         <v>74</v>
       </c>
@@ -8147,13 +8143,13 @@
       <c r="E16" s="237">
         <v>1</v>
       </c>
-      <c r="F16" s="572"/>
+      <c r="F16" s="593"/>
       <c r="G16" s="374" t="s">
         <v>506</v>
       </c>
       <c r="I16" s="20"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="575"/>
+      <c r="O16" s="627"/>
       <c r="R16" s="492" t="s">
         <v>185</v>
       </c>
@@ -8185,18 +8181,18 @@
       <c r="AM16" s="485" t="s">
         <v>324</v>
       </c>
-      <c r="AN16" s="591"/>
+      <c r="AN16" s="588"/>
       <c r="AP16" s="76" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="572"/>
+      <c r="F17" s="593"/>
       <c r="I17" s="20"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="575"/>
+      <c r="O17" s="627"/>
       <c r="Q17" s="21" t="s">
         <v>560</v>
       </c>
@@ -8241,7 +8237,7 @@
       <c r="AK17" s="272"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="485"/>
-      <c r="AN17" s="591"/>
+      <c r="AN17" s="588"/>
       <c r="AO17" s="214" t="s">
         <v>516</v>
       </c>
@@ -8265,21 +8261,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="572"/>
+      <c r="F18" s="593"/>
       <c r="G18" s="374" t="s">
         <v>557</v>
       </c>
       <c r="I18" s="20"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="575"/>
+      <c r="O18" s="627"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="567" t="s">
+      <c r="R18" s="621" t="s">
         <v>565</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="611" t="s">
+      <c r="U18" s="566" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -8300,7 +8296,7 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="272"/>
-      <c r="AF18" s="580" t="s">
+      <c r="AF18" s="602" t="s">
         <v>493</v>
       </c>
       <c r="AG18" s="272"/>
@@ -8312,19 +8308,19 @@
       <c r="AK18" s="272"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="485"/>
-      <c r="AN18" s="591"/>
+      <c r="AN18" s="588"/>
       <c r="AP18" s="76" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="572"/>
-      <c r="O19" s="575"/>
-      <c r="R19" s="568"/>
+      <c r="F19" s="593"/>
+      <c r="O19" s="627"/>
+      <c r="R19" s="622"/>
       <c r="S19" s="30" t="s">
         <v>563</v>
       </c>
-      <c r="U19" s="612"/>
+      <c r="U19" s="567"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="488" t="s">
@@ -8339,7 +8335,7 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="272"/>
-      <c r="AF19" s="580"/>
+      <c r="AF19" s="602"/>
       <c r="AG19" s="272"/>
       <c r="AH19" s="272"/>
       <c r="AI19" s="70"/>
@@ -8349,7 +8345,7 @@
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="485"/>
-      <c r="AN19" s="591"/>
+      <c r="AN19" s="588"/>
       <c r="AP19" s="76" t="s">
         <v>486</v>
       </c>
@@ -8370,18 +8366,18 @@
       <c r="E20" s="494">
         <v>-1</v>
       </c>
-      <c r="F20" s="572"/>
+      <c r="F20" s="593"/>
       <c r="G20" s="374" t="s">
         <v>509</v>
       </c>
-      <c r="O20" s="575"/>
-      <c r="Q20" s="577" t="s">
+      <c r="O20" s="627"/>
+      <c r="Q20" s="629" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="461" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="613"/>
+      <c r="U20" s="568"/>
       <c r="W20" s="462"/>
       <c r="X20" s="489" t="s">
         <v>175</v>
@@ -8411,7 +8407,7 @@
       <c r="AM20" s="427" t="s">
         <v>254</v>
       </c>
-      <c r="AN20" s="591"/>
+      <c r="AN20" s="588"/>
       <c r="AO20" s="375" t="s">
         <v>478</v>
       </c>
@@ -8435,12 +8431,12 @@
       <c r="E21" s="281">
         <v>1</v>
       </c>
-      <c r="F21" s="572"/>
-      <c r="O21" s="575"/>
-      <c r="Q21" s="578"/>
+      <c r="F21" s="593"/>
+      <c r="O21" s="627"/>
+      <c r="Q21" s="630"/>
       <c r="T21" s="479"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="608"/>
+      <c r="V21" s="563"/>
       <c r="W21" s="483" t="s">
         <v>176</v>
       </c>
@@ -8478,14 +8474,14 @@
       <c r="AM21" s="485" t="s">
         <v>575</v>
       </c>
-      <c r="AN21" s="591"/>
+      <c r="AN21" s="588"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="572"/>
+      <c r="F22" s="593"/>
       <c r="G22" s="374" t="s">
         <v>507</v>
       </c>
-      <c r="O22" s="575"/>
+      <c r="O22" s="627"/>
       <c r="R22" s="491" t="s">
         <v>44</v>
       </c>
@@ -8493,7 +8489,7 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="609"/>
+      <c r="V22" s="564"/>
       <c r="W22" s="483" t="s">
         <v>176</v>
       </c>
@@ -8511,7 +8507,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="580" t="s">
+      <c r="AJ22" s="602" t="s">
         <v>490</v>
       </c>
       <c r="AK22" s="272"/>
@@ -8519,7 +8515,7 @@
         <v>496</v>
       </c>
       <c r="AM22" s="318"/>
-      <c r="AN22" s="591"/>
+      <c r="AN22" s="588"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="244" t="s">
@@ -8537,16 +8533,16 @@
       <c r="E23" s="238">
         <v>1</v>
       </c>
-      <c r="F23" s="572"/>
-      <c r="O23" s="575"/>
-      <c r="Q23" s="577" t="s">
+      <c r="F23" s="593"/>
+      <c r="O23" s="627"/>
+      <c r="Q23" s="629" t="s">
         <v>145</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="477" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="609"/>
+      <c r="V23" s="564"/>
       <c r="W23" s="148"/>
       <c r="X23" s="486" t="s">
         <v>189</v>
@@ -8562,13 +8558,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="580"/>
+      <c r="AJ23" s="602"/>
       <c r="AK23" s="272"/>
       <c r="AL23" s="80" t="s">
         <v>526</v>
       </c>
       <c r="AM23" s="318"/>
-      <c r="AN23" s="591"/>
+      <c r="AN23" s="588"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="497" t="s">
@@ -8586,17 +8582,17 @@
       <c r="E24" s="493">
         <v>1</v>
       </c>
-      <c r="F24" s="572"/>
+      <c r="F24" s="593"/>
       <c r="G24" s="61" t="s">
         <v>508</v>
       </c>
-      <c r="O24" s="575"/>
-      <c r="Q24" s="578"/>
+      <c r="O24" s="627"/>
+      <c r="Q24" s="630"/>
       <c r="T24" s="17"/>
       <c r="U24" s="240" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="609"/>
+      <c r="V24" s="564"/>
       <c r="W24" s="148"/>
       <c r="X24" s="486" t="s">
         <v>186</v>
@@ -8620,11 +8616,11 @@
         <v>481</v>
       </c>
       <c r="AM24" s="318"/>
-      <c r="AN24" s="591"/>
+      <c r="AN24" s="588"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="572"/>
-      <c r="O25" s="575"/>
+      <c r="F25" s="593"/>
+      <c r="O25" s="627"/>
       <c r="P25" s="214" t="s">
         <v>285</v>
       </c>
@@ -8637,7 +8633,7 @@
       <c r="U25" s="454" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="610"/>
+      <c r="V25" s="565"/>
       <c r="W25" s="148"/>
       <c r="X25" s="486" t="s">
         <v>190</v>
@@ -8659,7 +8655,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="318"/>
-      <c r="AN25" s="591"/>
+      <c r="AN25" s="588"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="244" t="s">
@@ -8677,16 +8673,16 @@
       <c r="E26" s="424">
         <v>1</v>
       </c>
-      <c r="F26" s="572"/>
+      <c r="F26" s="593"/>
       <c r="G26" s="374" t="s">
         <v>505</v>
       </c>
-      <c r="O26" s="575"/>
-      <c r="P26" s="593" t="s">
+      <c r="O26" s="627"/>
+      <c r="P26" s="590" t="s">
         <v>551</v>
       </c>
-      <c r="Q26" s="594"/>
-      <c r="R26" s="569" t="s">
+      <c r="Q26" s="591"/>
+      <c r="R26" s="623" t="s">
         <v>564</v>
       </c>
       <c r="T26" s="183"/>
@@ -8725,7 +8721,7 @@
       <c r="AM26" s="499" t="s">
         <v>474</v>
       </c>
-      <c r="AN26" s="591"/>
+      <c r="AN26" s="588"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -8737,12 +8733,12 @@
       <c r="E27" s="281" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="573"/>
+      <c r="F27" s="625"/>
       <c r="G27" s="61" t="s">
         <v>574</v>
       </c>
-      <c r="O27" s="576"/>
-      <c r="R27" s="570"/>
+      <c r="O27" s="628"/>
+      <c r="R27" s="624"/>
       <c r="S27" s="478" t="s">
         <v>54</v>
       </c>
@@ -8772,10 +8768,48 @@
       <c r="AM27" s="427" t="s">
         <v>326</v>
       </c>
-      <c r="AN27" s="592"/>
+      <c r="AN27" s="589"/>
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="F2:F27"/>
+    <mergeCell ref="O10:O27"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="AI6:AI10"/>
+    <mergeCell ref="AF12:AF15"/>
+    <mergeCell ref="AG7:AG12"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="AN1:AN27"/>
+    <mergeCell ref="P26:Q26"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="M2:M9"/>
+    <mergeCell ref="O2:O9"/>
+    <mergeCell ref="P10:P13"/>
+    <mergeCell ref="AK6:AK7"/>
+    <mergeCell ref="AM12:AM15"/>
+    <mergeCell ref="AF18:AF19"/>
+    <mergeCell ref="AJ18:AJ19"/>
+    <mergeCell ref="Y1:Y27"/>
+    <mergeCell ref="AJ22:AJ23"/>
+    <mergeCell ref="AK9:AK10"/>
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="R2:R3"/>
     <mergeCell ref="V21:V25"/>
     <mergeCell ref="U18:U20"/>
     <mergeCell ref="C2:C3"/>
@@ -8792,44 +8826,6 @@
     <mergeCell ref="B11:B12"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="AN1:AN27"/>
-    <mergeCell ref="P26:Q26"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="M2:M9"/>
-    <mergeCell ref="O2:O9"/>
-    <mergeCell ref="P10:P13"/>
-    <mergeCell ref="AK6:AK7"/>
-    <mergeCell ref="AM12:AM15"/>
-    <mergeCell ref="AF18:AF19"/>
-    <mergeCell ref="AJ18:AJ19"/>
-    <mergeCell ref="Y1:Y27"/>
-    <mergeCell ref="AJ22:AJ23"/>
-    <mergeCell ref="AK9:AK10"/>
-    <mergeCell ref="AD3:AD4"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="AI6:AI10"/>
-    <mergeCell ref="AF12:AF15"/>
-    <mergeCell ref="AG7:AG12"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="AD12:AD15"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="F2:F27"/>
-    <mergeCell ref="O10:O27"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="H12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8839,8 +8835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AN37"/>
   <sheetViews>
-    <sheetView topLeftCell="P18" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+    <sheetView topLeftCell="O5" workbookViewId="0">
+      <selection activeCell="AG25" sqref="AG25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8930,13 +8926,13 @@
       <c r="T1" s="559" t="s">
         <v>236</v>
       </c>
-      <c r="U1" s="636" t="s">
+      <c r="U1" s="647" t="s">
         <v>237</v>
       </c>
-      <c r="V1" s="638" t="s">
+      <c r="V1" s="649" t="s">
         <v>459</v>
       </c>
-      <c r="W1" s="639"/>
+      <c r="W1" s="650"/>
       <c r="X1" s="324">
         <f>68-(S8+W3+V3+Q3)</f>
         <v>0</v>
@@ -8952,40 +8948,40 @@
       <c r="AB1" s="320" t="s">
         <v>44</v>
       </c>
-      <c r="AC1" s="640" t="s">
+      <c r="AC1" s="651" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="641"/>
-      <c r="AE1" s="642"/>
-      <c r="AF1" s="643" t="s">
+      <c r="AD1" s="652"/>
+      <c r="AE1" s="653"/>
+      <c r="AF1" s="654" t="s">
         <v>298</v>
       </c>
-      <c r="AG1" s="644"/>
-      <c r="AH1" s="645"/>
-      <c r="AI1" s="632" t="s">
+      <c r="AG1" s="655"/>
+      <c r="AH1" s="656"/>
+      <c r="AI1" s="643" t="s">
         <v>462</v>
       </c>
-      <c r="AJ1" s="633"/>
-      <c r="AK1" s="634"/>
+      <c r="AJ1" s="644"/>
+      <c r="AK1" s="645"/>
       <c r="AN1" s="112"/>
     </row>
     <row r="2" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F2" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="J2" s="646">
+      <c r="J2" s="635">
         <f>SUM(J5:J30)</f>
         <v>0</v>
       </c>
-      <c r="K2" s="648">
+      <c r="K2" s="637">
         <f>SUM(K4:K29)</f>
-        <v>6</v>
-      </c>
-      <c r="L2" s="650">
+        <v>4</v>
+      </c>
+      <c r="L2" s="639">
         <f>SUM(L4:L29)</f>
-        <v>6</v>
-      </c>
-      <c r="M2" s="587">
+        <v>5</v>
+      </c>
+      <c r="M2" s="614">
         <f>SUM(K30:K37)* (-1)</f>
         <v>1</v>
       </c>
@@ -9004,11 +9000,11 @@
       <c r="R2" s="61" t="s">
         <v>221</v>
       </c>
-      <c r="S2" s="652" t="s">
+      <c r="S2" s="641" t="s">
         <v>239</v>
       </c>
-      <c r="T2" s="635"/>
-      <c r="U2" s="637"/>
+      <c r="T2" s="646"/>
+      <c r="U2" s="648"/>
       <c r="V2" s="61" t="s">
         <v>456</v>
       </c>
@@ -9068,10 +9064,10 @@
       </c>
     </row>
     <row r="3" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J3" s="647"/>
-      <c r="K3" s="649"/>
-      <c r="L3" s="651"/>
-      <c r="M3" s="588"/>
+      <c r="J3" s="636"/>
+      <c r="K3" s="638"/>
+      <c r="L3" s="640"/>
+      <c r="M3" s="615"/>
       <c r="N3" s="177">
         <f>(J2+K2)-W3</f>
         <v>0</v>
@@ -9081,13 +9077,13 @@
       </c>
       <c r="Q3" s="150">
         <f>SUM(Q4:Q29)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="R3" s="159">
         <f>SUM(R4:R29)</f>
-        <v>42</v>
-      </c>
-      <c r="S3" s="653"/>
+        <v>43</v>
+      </c>
+      <c r="S3" s="642"/>
       <c r="T3" s="560"/>
       <c r="U3" s="331">
         <f>R3+V3+W3+Q3</f>
@@ -9099,7 +9095,7 @@
       </c>
       <c r="W3" s="187">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="X3" s="59">
         <f t="shared" si="0"/>
@@ -9107,15 +9103,15 @@
       </c>
       <c r="Y3" s="66">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Z3" s="66">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="AA3" s="66">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AB3" s="66">
         <f t="shared" ref="AB3:AK3" si="1">SUM(AB4:AB29)</f>
@@ -9123,7 +9119,7 @@
       </c>
       <c r="AC3" s="66">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AD3" s="66">
         <f t="shared" si="1"/>
@@ -9135,7 +9131,7 @@
       </c>
       <c r="AF3" s="66">
         <f>SUM(AF4:AF29)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AG3" s="412">
         <f t="shared" si="1"/>
@@ -9143,19 +9139,19 @@
       </c>
       <c r="AH3" s="100">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AI3" s="100">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AJ3" s="329">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AK3" s="330">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AN3" s="112"/>
     </row>
@@ -9189,7 +9185,7 @@
         <f>AA4</f>
         <v>0</v>
       </c>
-      <c r="M4" s="654" t="s">
+      <c r="M4" s="632" t="s">
         <v>200</v>
       </c>
       <c r="N4" s="20"/>
@@ -9268,7 +9264,7 @@
         <f>AA5</f>
         <v>0</v>
       </c>
-      <c r="M5" s="655"/>
+      <c r="M5" s="633"/>
       <c r="N5" s="20"/>
       <c r="O5" s="2" t="s">
         <v>347</v>
@@ -9356,7 +9352,7 @@
         <f>AA6</f>
         <v>0</v>
       </c>
-      <c r="M6" s="655"/>
+      <c r="M6" s="633"/>
       <c r="N6" s="19" t="s">
         <v>342</v>
       </c>
@@ -9446,7 +9442,7 @@
         <f t="shared" ref="L7:L37" si="10">AA7</f>
         <v>0</v>
       </c>
-      <c r="M7" s="655"/>
+      <c r="M7" s="633"/>
       <c r="N7" s="20"/>
       <c r="O7" s="2" t="s">
         <v>342</v>
@@ -9554,7 +9550,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M8" s="655"/>
+      <c r="M8" s="633"/>
       <c r="N8" s="21" t="s">
         <v>238</v>
       </c>
@@ -9572,7 +9568,7 @@
       </c>
       <c r="S8" s="340">
         <f>R3</f>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="T8" s="17"/>
       <c r="U8" s="348"/>
@@ -9640,7 +9636,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M9" s="655"/>
+      <c r="M9" s="633"/>
       <c r="N9" s="21" t="s">
         <v>342</v>
       </c>
@@ -9740,7 +9736,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M10" s="655"/>
+      <c r="M10" s="633"/>
       <c r="N10" s="20"/>
       <c r="O10" s="2" t="s">
         <v>347</v>
@@ -9819,7 +9815,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M11" s="655"/>
+      <c r="M11" s="633"/>
       <c r="N11" s="21" t="s">
         <v>342</v>
       </c>
@@ -9881,7 +9877,7 @@
       <c r="AN11" s="112"/>
     </row>
     <row r="12" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="623" t="s">
+      <c r="A12" s="578" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
@@ -9890,7 +9886,7 @@
       <c r="C12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="577" t="s">
+      <c r="E12" s="629" t="s">
         <v>57</v>
       </c>
       <c r="G12" s="277">
@@ -9910,7 +9906,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="M12" s="655"/>
+      <c r="M12" s="633"/>
       <c r="N12" s="21" t="s">
         <v>342</v>
       </c>
@@ -9984,14 +9980,14 @@
       </c>
     </row>
     <row r="13" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="625"/>
+      <c r="A13" s="580"/>
       <c r="B13" s="153">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="578"/>
+      <c r="E13" s="630"/>
       <c r="F13" s="177">
         <v>0</v>
       </c>
@@ -10012,7 +10008,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M13" s="655"/>
+      <c r="M13" s="633"/>
       <c r="N13" s="21" t="s">
         <v>342</v>
       </c>
@@ -10087,7 +10083,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M14" s="655"/>
+      <c r="M14" s="633"/>
       <c r="N14" s="20"/>
       <c r="O14" s="210" t="s">
         <v>346</v>
@@ -10170,7 +10166,7 @@
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="M15" s="655"/>
+      <c r="M15" s="633"/>
       <c r="N15" s="20"/>
       <c r="O15" s="210" t="s">
         <v>346</v>
@@ -10257,7 +10253,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="M16" s="655"/>
+      <c r="M16" s="633"/>
       <c r="N16" s="21" t="s">
         <v>342</v>
       </c>
@@ -10344,7 +10340,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M17" s="655"/>
+      <c r="M17" s="633"/>
       <c r="N17" s="20"/>
       <c r="O17" s="2" t="s">
         <v>348</v>
@@ -10427,7 +10423,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M18" s="655"/>
+      <c r="M18" s="633"/>
       <c r="N18" s="21" t="s">
         <v>342</v>
       </c>
@@ -10514,7 +10510,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M19" s="655"/>
+      <c r="M19" s="633"/>
       <c r="N19" s="20"/>
       <c r="O19" s="2" t="s">
         <v>341</v>
@@ -10603,11 +10599,11 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M20" s="656"/>
+      <c r="M20" s="634"/>
       <c r="N20" s="529" t="s">
         <v>342</v>
       </c>
-      <c r="O20" s="579"/>
+      <c r="O20" s="631"/>
       <c r="P20" s="334" t="s">
         <v>86</v>
       </c>
@@ -10691,11 +10687,11 @@
       </c>
       <c r="J21" s="365"/>
       <c r="K21" s="107">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L21" s="311">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N21" s="20"/>
       <c r="O21" s="2" t="s">
@@ -10705,10 +10701,10 @@
         <v>250</v>
       </c>
       <c r="Q21" s="164">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R21" s="157">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S21" s="338">
         <v>-1</v>
@@ -10718,50 +10714,50 @@
       <c r="V21" s="343"/>
       <c r="W21" s="190">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X21" s="314"/>
       <c r="Y21" s="117">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z21" s="308">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AA21" s="308">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB21" s="308">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AC21" s="312">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD21" s="318"/>
       <c r="AE21" s="314"/>
       <c r="AF21" s="314">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG21" s="373">
         <v>0</v>
       </c>
       <c r="AH21" s="158">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI21" s="326">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ21" s="327">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK21" s="328">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL21" s="6" t="s">
         <v>84</v>
@@ -10848,7 +10844,7 @@
       <c r="AN22" s="112"/>
     </row>
     <row r="23" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E23" s="630" t="s">
+      <c r="E23" s="585" t="s">
         <v>294</v>
       </c>
       <c r="F23" s="185">
@@ -10934,7 +10930,7 @@
       <c r="C24" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E24" s="631"/>
+      <c r="E24" s="586"/>
       <c r="F24" s="177"/>
       <c r="I24" s="431" t="s">
         <v>301</v>
@@ -10952,7 +10948,7 @@
       <c r="N24" s="529" t="s">
         <v>342</v>
       </c>
-      <c r="O24" s="579"/>
+      <c r="O24" s="631"/>
       <c r="P24" s="334" t="s">
         <v>254</v>
       </c>
@@ -12022,23 +12018,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="AI1:AK1"/>
+    <mergeCell ref="T1:T3"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AF1:AH1"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="S2:S3"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="N20:O20"/>
     <mergeCell ref="E23:E24"/>
     <mergeCell ref="N24:O24"/>
     <mergeCell ref="M4:M20"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="AI1:AK1"/>
-    <mergeCell ref="T1:T3"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="AC1:AE1"/>
-    <mergeCell ref="AF1:AH1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12075,12 +12071,12 @@
       <c r="B1" s="529" t="s">
         <v>317</v>
       </c>
-      <c r="C1" s="579"/>
+      <c r="C1" s="631"/>
       <c r="D1" s="214"/>
       <c r="J1" s="529" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="579"/>
+      <c r="K1" s="631"/>
       <c r="L1" s="205" t="s">
         <v>337</v>
       </c>
@@ -12471,7 +12467,7 @@
       <c r="V1" s="529" t="s">
         <v>71</v>
       </c>
-      <c r="W1" s="579"/>
+      <c r="W1" s="631"/>
       <c r="X1" s="62" t="s">
         <v>102</v>
       </c>
@@ -12490,7 +12486,7 @@
       <c r="AC1" s="116" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="670" t="s">
+      <c r="AD1" s="677" t="s">
         <v>213</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -12507,10 +12503,10 @@
       <c r="E2" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="669" t="s">
+      <c r="F2" s="708" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="697" t="s">
+      <c r="G2" s="665" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -12538,10 +12534,10 @@
       <c r="U2" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="V2" s="638" t="s">
+      <c r="V2" s="649" t="s">
         <v>121</v>
       </c>
-      <c r="W2" s="639"/>
+      <c r="W2" s="650"/>
       <c r="X2" s="64" t="s">
         <v>110</v>
       </c>
@@ -12560,7 +12556,7 @@
       <c r="AC2" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="AD2" s="671"/>
+      <c r="AD2" s="678"/>
       <c r="AE2" s="64" t="s">
         <v>99</v>
       </c>
@@ -12579,8 +12575,8 @@
       <c r="E3" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="627"/>
-      <c r="G3" s="698"/>
+      <c r="F3" s="582"/>
+      <c r="G3" s="666"/>
       <c r="H3" s="40" t="s">
         <v>81</v>
       </c>
@@ -12591,13 +12587,13 @@
         <v>82</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="707" t="s">
+      <c r="O3" s="675" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="689" t="s">
+      <c r="P3" s="696" t="s">
         <v>219</v>
       </c>
-      <c r="Q3" s="690"/>
+      <c r="Q3" s="697"/>
       <c r="S3" s="57" t="s">
         <v>220</v>
       </c>
@@ -12607,15 +12603,15 @@
       <c r="W3" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="AD3" s="671"/>
+      <c r="AD3" s="678"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="698"/>
+      <c r="G4" s="666"/>
       <c r="H4" s="6"/>
       <c r="L4" s="660" t="s">
         <v>83</v>
       </c>
-      <c r="O4" s="708"/>
+      <c r="O4" s="676"/>
       <c r="T4" s="55" t="s">
         <v>98</v>
       </c>
@@ -12629,8 +12625,8 @@
         <v>195</v>
       </c>
       <c r="Z4" s="530"/>
-      <c r="AA4" s="579"/>
-      <c r="AD4" s="671"/>
+      <c r="AA4" s="631"/>
+      <c r="AD4" s="678"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -12645,21 +12641,21 @@
       <c r="F5" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="698"/>
+      <c r="G5" s="666"/>
       <c r="H5" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="676" t="s">
+      <c r="K5" s="683" t="s">
         <v>217</v>
       </c>
-      <c r="L5" s="691"/>
+      <c r="L5" s="698"/>
       <c r="M5" s="2" t="s">
         <v>215</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>214</v>
       </c>
-      <c r="O5" s="708"/>
+      <c r="O5" s="676"/>
       <c r="P5" s="108" t="s">
         <v>216</v>
       </c>
@@ -12675,11 +12671,11 @@
       <c r="U5" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="Y5" s="679" t="s">
+      <c r="Y5" s="686" t="s">
         <v>287</v>
       </c>
-      <c r="Z5" s="680"/>
-      <c r="AD5" s="671"/>
+      <c r="Z5" s="687"/>
+      <c r="AD5" s="678"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -12689,16 +12685,16 @@
       <c r="E6" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="698"/>
+      <c r="G6" s="666"/>
       <c r="H6" s="46" t="s">
         <v>81</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="677"/>
-      <c r="L6" s="691"/>
-      <c r="O6" s="708"/>
+      <c r="K6" s="684"/>
+      <c r="L6" s="698"/>
+      <c r="O6" s="676"/>
       <c r="S6" s="104" t="s">
         <v>20</v>
       </c>
@@ -12711,20 +12707,20 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="671"/>
+      <c r="AD6" s="678"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="698"/>
+      <c r="G7" s="666"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="677"/>
-      <c r="L7" s="691"/>
+      <c r="K7" s="684"/>
+      <c r="L7" s="698"/>
       <c r="N7" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="O7" s="708"/>
+      <c r="O7" s="676"/>
       <c r="P7" s="73"/>
-      <c r="AD7" s="671"/>
+      <c r="AD7" s="678"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -12737,7 +12733,7 @@
       <c r="F8" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="698"/>
+      <c r="G8" s="666"/>
       <c r="H8" s="50" t="s">
         <v>76</v>
       </c>
@@ -12747,41 +12743,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="677"/>
-      <c r="L8" s="691"/>
-      <c r="O8" s="708"/>
+      <c r="K8" s="684"/>
+      <c r="L8" s="698"/>
+      <c r="O8" s="676"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="673" t="s">
+      <c r="S8" s="680" t="s">
         <v>212</v>
       </c>
-      <c r="T8" s="674"/>
-      <c r="U8" s="674"/>
-      <c r="V8" s="674"/>
-      <c r="W8" s="674"/>
-      <c r="X8" s="674"/>
-      <c r="Y8" s="674"/>
-      <c r="Z8" s="674"/>
-      <c r="AA8" s="674"/>
-      <c r="AB8" s="674"/>
-      <c r="AC8" s="675"/>
-      <c r="AD8" s="671"/>
+      <c r="T8" s="681"/>
+      <c r="U8" s="681"/>
+      <c r="V8" s="681"/>
+      <c r="W8" s="681"/>
+      <c r="X8" s="681"/>
+      <c r="Y8" s="681"/>
+      <c r="Z8" s="681"/>
+      <c r="AA8" s="681"/>
+      <c r="AB8" s="681"/>
+      <c r="AC8" s="682"/>
+      <c r="AD8" s="678"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="663"/>
-      <c r="G9" s="698"/>
+      <c r="C9" s="702"/>
+      <c r="G9" s="666"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="677"/>
-      <c r="L9" s="701" t="s">
+      <c r="K9" s="684"/>
+      <c r="L9" s="669" t="s">
         <v>218</v>
       </c>
-      <c r="M9" s="702"/>
-      <c r="N9" s="703"/>
-      <c r="O9" s="708"/>
+      <c r="M9" s="670"/>
+      <c r="N9" s="671"/>
+      <c r="O9" s="676"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="671"/>
+      <c r="AD9" s="678"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="664"/>
+      <c r="C10" s="703"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>88</v>
@@ -12789,7 +12785,7 @@
       <c r="F10" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="698"/>
+      <c r="G10" s="666"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>81</v>
@@ -12797,33 +12793,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="677"/>
-      <c r="M10" s="666" t="s">
+      <c r="K10" s="684"/>
+      <c r="M10" s="705" t="s">
         <v>90</v>
       </c>
-      <c r="N10" s="667"/>
-      <c r="O10" s="667"/>
-      <c r="P10" s="667"/>
-      <c r="Q10" s="667"/>
-      <c r="R10" s="667"/>
-      <c r="S10" s="667"/>
-      <c r="T10" s="667"/>
-      <c r="U10" s="667"/>
-      <c r="V10" s="667"/>
-      <c r="W10" s="667"/>
-      <c r="X10" s="667"/>
-      <c r="Y10" s="667"/>
-      <c r="Z10" s="667"/>
-      <c r="AA10" s="667"/>
-      <c r="AB10" s="667"/>
-      <c r="AC10" s="668"/>
-      <c r="AD10" s="671"/>
+      <c r="N10" s="706"/>
+      <c r="O10" s="706"/>
+      <c r="P10" s="706"/>
+      <c r="Q10" s="706"/>
+      <c r="R10" s="706"/>
+      <c r="S10" s="706"/>
+      <c r="T10" s="706"/>
+      <c r="U10" s="706"/>
+      <c r="V10" s="706"/>
+      <c r="W10" s="706"/>
+      <c r="X10" s="706"/>
+      <c r="Y10" s="706"/>
+      <c r="Z10" s="706"/>
+      <c r="AA10" s="706"/>
+      <c r="AB10" s="706"/>
+      <c r="AC10" s="707"/>
+      <c r="AD10" s="678"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="665"/>
-      <c r="G11" s="698"/>
+      <c r="C11" s="704"/>
+      <c r="G11" s="666"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="677"/>
+      <c r="K11" s="684"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -12831,17 +12827,17 @@
       <c r="Y11" s="68" t="s">
         <v>121</v>
       </c>
-      <c r="Z11" s="687" t="s">
+      <c r="Z11" s="694" t="s">
         <v>121</v>
       </c>
-      <c r="AA11" s="688"/>
+      <c r="AA11" s="695"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>121</v>
       </c>
-      <c r="AD11" s="671"/>
+      <c r="AD11" s="678"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -12854,7 +12850,7 @@
       <c r="F12" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="698"/>
+      <c r="G12" s="666"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>81</v>
@@ -12862,8 +12858,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="677"/>
-      <c r="L12" s="692" t="s">
+      <c r="K12" s="684"/>
+      <c r="L12" s="699" t="s">
         <v>93</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -12894,25 +12890,25 @@
         <v>116</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="681" t="s">
+      <c r="AA12" s="688" t="s">
         <v>126</v>
       </c>
-      <c r="AB12" s="682"/>
+      <c r="AB12" s="689"/>
       <c r="AC12" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="AD12" s="671"/>
+      <c r="AD12" s="678"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="663"/>
-      <c r="G13" s="698"/>
-      <c r="K13" s="677"/>
-      <c r="L13" s="693"/>
+      <c r="C13" s="702"/>
+      <c r="G13" s="666"/>
+      <c r="K13" s="684"/>
+      <c r="L13" s="700"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="700" t="s">
+      <c r="Q13" s="668" t="s">
         <v>210</v>
       </c>
-      <c r="R13" s="594"/>
+      <c r="R13" s="591"/>
       <c r="S13" s="525"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
@@ -12921,17 +12917,17 @@
       <c r="X13" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="AA13" s="683"/>
-      <c r="AB13" s="684"/>
-      <c r="AD13" s="671"/>
+      <c r="AA13" s="690"/>
+      <c r="AB13" s="691"/>
+      <c r="AD13" s="678"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="C14" s="665"/>
+      <c r="C14" s="704"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="698"/>
+      <c r="G14" s="666"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -12939,8 +12935,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="677"/>
-      <c r="L14" s="693"/>
+      <c r="K14" s="684"/>
+      <c r="L14" s="700"/>
       <c r="M14" s="21" t="s">
         <v>111</v>
       </c>
@@ -12961,9 +12957,9 @@
       <c r="Y14" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="AA14" s="683"/>
-      <c r="AB14" s="684"/>
-      <c r="AD14" s="671"/>
+      <c r="AA14" s="690"/>
+      <c r="AB14" s="691"/>
+      <c r="AD14" s="678"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -12978,19 +12974,19 @@
       <c r="F15" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="698"/>
+      <c r="G15" s="666"/>
       <c r="H15" s="2" t="s">
         <v>81</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="K15" s="677"/>
-      <c r="L15" s="694"/>
-      <c r="Q15" s="700" t="s">
+      <c r="K15" s="684"/>
+      <c r="L15" s="701"/>
+      <c r="Q15" s="668" t="s">
         <v>211</v>
       </c>
-      <c r="R15" s="594"/>
+      <c r="R15" s="591"/>
       <c r="S15" s="525"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
@@ -12999,14 +12995,14 @@
       <c r="X15" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AA15" s="683"/>
-      <c r="AB15" s="684"/>
-      <c r="AD15" s="671"/>
+      <c r="AA15" s="690"/>
+      <c r="AB15" s="691"/>
+      <c r="AD15" s="678"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="698"/>
-      <c r="K16" s="677"/>
+      <c r="G16" s="666"/>
+      <c r="K16" s="684"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>109</v>
@@ -13025,24 +13021,24 @@
       <c r="Z16" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="AA16" s="683"/>
-      <c r="AB16" s="684"/>
-      <c r="AD16" s="671"/>
+      <c r="AA16" s="690"/>
+      <c r="AB16" s="691"/>
+      <c r="AD16" s="678"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F17" s="695" t="s">
+      <c r="F17" s="663" t="s">
         <v>96</v>
       </c>
-      <c r="G17" s="698"/>
+      <c r="G17" s="666"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>81</v>
       </c>
-      <c r="K17" s="677"/>
+      <c r="K17" s="684"/>
       <c r="S17" s="525"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
@@ -13050,9 +13046,9 @@
       <c r="X17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AA17" s="683"/>
-      <c r="AB17" s="684"/>
-      <c r="AD17" s="671"/>
+      <c r="AA17" s="690"/>
+      <c r="AB17" s="691"/>
+      <c r="AD17" s="678"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -13062,15 +13058,15 @@
       <c r="E18" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="696"/>
-      <c r="G18" s="698"/>
+      <c r="F18" s="664"/>
+      <c r="G18" s="666"/>
       <c r="H18" s="108" t="s">
         <v>76</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="K18" s="677"/>
+      <c r="K18" s="684"/>
       <c r="O18" s="64" t="s">
         <v>115</v>
       </c>
@@ -13081,42 +13077,39 @@
       <c r="X18" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA18" s="685"/>
-      <c r="AB18" s="686"/>
-      <c r="AD18" s="671"/>
+      <c r="AA18" s="692"/>
+      <c r="AB18" s="693"/>
+      <c r="AD18" s="678"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>209</v>
       </c>
-      <c r="G19" s="699"/>
-      <c r="K19" s="678"/>
+      <c r="G19" s="667"/>
+      <c r="K19" s="685"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="704" t="s">
+      <c r="R19" s="672" t="s">
         <v>124</v>
       </c>
-      <c r="S19" s="705"/>
-      <c r="T19" s="706"/>
+      <c r="S19" s="673"/>
+      <c r="T19" s="674"/>
       <c r="V19" s="77" t="s">
         <v>115</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="AD19" s="672"/>
+      <c r="AD19" s="679"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G2:G19"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="S12:S18"/>
-    <mergeCell ref="O3:O9"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="M10:AC10"/>
+    <mergeCell ref="F2:F3"/>
     <mergeCell ref="AD1:AD19"/>
     <mergeCell ref="S8:AC8"/>
     <mergeCell ref="K5:K19"/>
@@ -13128,11 +13121,14 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="L12:L15"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="M10:AC10"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="S12:S18"/>
+    <mergeCell ref="O3:O9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
CNN Turk ShieldW Halted
CNN Turk ShieldW Halted
</commit_message>
<xml_diff>
--- a/System_2.1.2.xlsx
+++ b/System_2.1.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E2582D2-4BB5-431F-83EB-6D7F31BB1A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CDBC42-C7CC-4212-9E82-EF1B2547168C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BoardRW" sheetId="1" r:id="rId1"/>
@@ -4724,6 +4724,141 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4796,140 +4931,71 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="43" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="49" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="35" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
@@ -4940,130 +5006,43 @@
     <xf numFmtId="0" fontId="3" fillId="35" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="43" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5141,25 +5120,46 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -6310,8 +6310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB54FD83-008D-4F8B-87AC-83E7F70047CB}">
   <dimension ref="A1:W29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E10" workbookViewId="0">
-      <selection activeCell="V20" sqref="V20"/>
+    <sheetView topLeftCell="E11" workbookViewId="0">
+      <selection activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6575,7 +6575,7 @@
       <c r="D10" s="108"/>
       <c r="E10" s="68">
         <f>Boat!S8</f>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G10" s="525"/>
       <c r="I10" s="542"/>
@@ -7059,7 +7059,7 @@
       </c>
       <c r="Q29" s="457"/>
       <c r="R29" s="460">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="S29" s="521">
         <v>-1</v>
@@ -7068,7 +7068,7 @@
         <v>418</v>
       </c>
       <c r="V29">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="W29" s="6" t="s">
         <v>235</v>
@@ -7225,7 +7225,7 @@
         <v>517</v>
       </c>
       <c r="AM1" s="458"/>
-      <c r="AN1" s="587"/>
+      <c r="AN1" s="590"/>
       <c r="AO1" s="375" t="s">
         <v>487</v>
       </c>
@@ -7234,23 +7234,23 @@
       </c>
     </row>
     <row r="2" spans="1:43" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="569">
+      <c r="A2" s="614">
         <f ca="1">TODAY()</f>
         <v>45275</v>
       </c>
-      <c r="B2" s="571" t="s">
+      <c r="B2" s="616" t="s">
         <v>379</v>
       </c>
       <c r="C2" s="561" t="s">
         <v>365</v>
       </c>
-      <c r="D2" s="573" t="s">
+      <c r="D2" s="618" t="s">
         <v>362</v>
       </c>
-      <c r="E2" s="617" t="s">
+      <c r="E2" s="563" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="592" t="s">
+      <c r="F2" s="571" t="s">
         <v>103</v>
       </c>
       <c r="G2" s="446" t="s">
@@ -7263,17 +7263,17 @@
       <c r="J2" s="81" t="s">
         <v>77</v>
       </c>
-      <c r="K2" s="619" t="s">
+      <c r="K2" s="565" t="s">
         <v>349</v>
       </c>
-      <c r="L2" s="620"/>
-      <c r="M2" s="592" t="s">
+      <c r="L2" s="566"/>
+      <c r="M2" s="571" t="s">
         <v>103</v>
       </c>
       <c r="N2" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="596" t="s">
+      <c r="O2" s="597" t="s">
         <v>103</v>
       </c>
       <c r="P2" s="85" t="s">
@@ -7283,7 +7283,7 @@
         <v>144</v>
       </c>
       <c r="R2" s="524"/>
-      <c r="S2" s="609" t="s">
+      <c r="S2" s="584" t="s">
         <v>149</v>
       </c>
       <c r="T2" s="89"/>
@@ -7316,15 +7316,15 @@
         <v>481</v>
       </c>
       <c r="AM2" s="485"/>
-      <c r="AN2" s="588"/>
+      <c r="AN2" s="591"/>
     </row>
     <row r="3" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="570"/>
-      <c r="B3" s="572"/>
+      <c r="A3" s="615"/>
+      <c r="B3" s="617"/>
       <c r="C3" s="562"/>
-      <c r="D3" s="574"/>
-      <c r="E3" s="618"/>
-      <c r="F3" s="593"/>
+      <c r="D3" s="619"/>
+      <c r="E3" s="564"/>
+      <c r="F3" s="572"/>
       <c r="G3" s="447" t="s">
         <v>28</v>
       </c>
@@ -7343,17 +7343,17 @@
       <c r="L3" s="211" t="s">
         <v>108</v>
       </c>
-      <c r="M3" s="593"/>
+      <c r="M3" s="572"/>
       <c r="N3" s="69" t="s">
         <v>147</v>
       </c>
-      <c r="O3" s="597"/>
+      <c r="O3" s="598"/>
       <c r="P3" s="2" t="s">
         <v>155</v>
       </c>
       <c r="Q3" s="562"/>
       <c r="R3" s="526"/>
-      <c r="S3" s="610"/>
+      <c r="S3" s="586"/>
       <c r="T3" s="89"/>
       <c r="U3" s="124"/>
       <c r="V3" s="120"/>
@@ -7370,7 +7370,7 @@
       <c r="AC3" s="100" t="s">
         <v>498</v>
       </c>
-      <c r="AD3" s="608" t="s">
+      <c r="AD3" s="581" t="s">
         <v>473</v>
       </c>
       <c r="AE3" s="272"/>
@@ -7382,13 +7382,13 @@
       <c r="AK3" s="272"/>
       <c r="AL3" s="16"/>
       <c r="AM3" s="485"/>
-      <c r="AN3" s="588"/>
+      <c r="AN3" s="591"/>
     </row>
     <row r="4" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="251" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="585" t="s">
+      <c r="B4" s="630" t="s">
         <v>382</v>
       </c>
       <c r="C4" s="561" t="s">
@@ -7400,7 +7400,7 @@
       <c r="E4" s="422">
         <v>1</v>
       </c>
-      <c r="F4" s="593"/>
+      <c r="F4" s="572"/>
       <c r="G4" s="427" t="s">
         <v>203</v>
       </c>
@@ -7417,11 +7417,11 @@
         <v>151</v>
       </c>
       <c r="L4" s="214"/>
-      <c r="M4" s="593"/>
+      <c r="M4" s="572"/>
       <c r="N4" s="179" t="s">
         <v>70</v>
       </c>
-      <c r="O4" s="597"/>
+      <c r="O4" s="598"/>
       <c r="P4" s="2" t="s">
         <v>192</v>
       </c>
@@ -7448,7 +7448,7 @@
       <c r="AA4" s="325"/>
       <c r="AB4" s="219"/>
       <c r="AC4" s="16"/>
-      <c r="AD4" s="608"/>
+      <c r="AD4" s="581"/>
       <c r="AE4" s="272"/>
       <c r="AF4" s="272"/>
       <c r="AG4" s="16"/>
@@ -7458,7 +7458,7 @@
       <c r="AK4" s="272"/>
       <c r="AL4" s="16"/>
       <c r="AM4" s="485"/>
-      <c r="AN4" s="588"/>
+      <c r="AN4" s="591"/>
       <c r="AO4" s="375" t="s">
         <v>91</v>
       </c>
@@ -7467,7 +7467,7 @@
       <c r="A5" s="559" t="s">
         <v>435</v>
       </c>
-      <c r="B5" s="586"/>
+      <c r="B5" s="631"/>
       <c r="C5" s="562"/>
       <c r="D5" s="61" t="s">
         <v>154</v>
@@ -7475,20 +7475,20 @@
       <c r="E5" s="423">
         <v>1</v>
       </c>
-      <c r="F5" s="593"/>
-      <c r="G5" s="577" t="s">
+      <c r="F5" s="572"/>
+      <c r="G5" s="622" t="s">
         <v>193</v>
       </c>
-      <c r="H5" s="577"/>
-      <c r="I5" s="577"/>
-      <c r="J5" s="577"/>
-      <c r="K5" s="577"/>
-      <c r="L5" s="578"/>
-      <c r="M5" s="593"/>
+      <c r="H5" s="622"/>
+      <c r="I5" s="622"/>
+      <c r="J5" s="622"/>
+      <c r="K5" s="622"/>
+      <c r="L5" s="623"/>
+      <c r="M5" s="572"/>
       <c r="N5" s="21">
         <v>8</v>
       </c>
-      <c r="O5" s="597"/>
+      <c r="O5" s="598"/>
       <c r="T5" s="89"/>
       <c r="U5" s="124"/>
       <c r="V5" s="120"/>
@@ -7519,24 +7519,24 @@
       <c r="AK5" s="272"/>
       <c r="AL5" s="80"/>
       <c r="AM5" s="485"/>
-      <c r="AN5" s="588"/>
+      <c r="AN5" s="591"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="560"/>
-      <c r="B6" s="583" t="s">
+      <c r="B6" s="628" t="s">
         <v>178</v>
       </c>
       <c r="C6" s="557"/>
       <c r="D6" s="558"/>
-      <c r="F6" s="593"/>
-      <c r="G6" s="579"/>
-      <c r="H6" s="579"/>
-      <c r="I6" s="579"/>
-      <c r="J6" s="579"/>
-      <c r="K6" s="579"/>
-      <c r="L6" s="580"/>
-      <c r="M6" s="593"/>
-      <c r="O6" s="597"/>
+      <c r="F6" s="572"/>
+      <c r="G6" s="624"/>
+      <c r="H6" s="624"/>
+      <c r="I6" s="624"/>
+      <c r="J6" s="624"/>
+      <c r="K6" s="624"/>
+      <c r="L6" s="625"/>
+      <c r="M6" s="572"/>
+      <c r="O6" s="598"/>
       <c r="T6" s="89"/>
       <c r="U6" s="124"/>
       <c r="V6" s="98" t="s">
@@ -7560,16 +7560,16 @@
       <c r="AF6" s="272"/>
       <c r="AG6" s="272"/>
       <c r="AH6" s="272"/>
-      <c r="AI6" s="602"/>
+      <c r="AI6" s="580"/>
       <c r="AJ6" s="498" t="s">
         <v>476</v>
       </c>
-      <c r="AK6" s="602" t="s">
+      <c r="AK6" s="580" t="s">
         <v>256</v>
       </c>
       <c r="AL6" s="272"/>
       <c r="AM6" s="485"/>
-      <c r="AN6" s="588"/>
+      <c r="AN6" s="591"/>
       <c r="AO6" s="375" t="s">
         <v>488</v>
       </c>
@@ -7578,7 +7578,7 @@
       <c r="A7" s="245" t="s">
         <v>554</v>
       </c>
-      <c r="B7" s="584"/>
+      <c r="B7" s="629"/>
       <c r="C7" s="212" t="s">
         <v>383</v>
       </c>
@@ -7588,7 +7588,7 @@
       <c r="E7" s="281">
         <v>3</v>
       </c>
-      <c r="F7" s="593"/>
+      <c r="F7" s="572"/>
       <c r="G7" s="448">
         <v>0</v>
       </c>
@@ -7607,8 +7607,8 @@
       <c r="L7" s="222">
         <v>0</v>
       </c>
-      <c r="M7" s="593"/>
-      <c r="O7" s="597"/>
+      <c r="M7" s="572"/>
+      <c r="O7" s="598"/>
       <c r="R7" s="99" t="s">
         <v>44</v>
       </c>
@@ -7632,18 +7632,18 @@
       <c r="AD7" s="16"/>
       <c r="AE7" s="272"/>
       <c r="AF7" s="272"/>
-      <c r="AG7" s="608" t="s">
+      <c r="AG7" s="581" t="s">
         <v>472</v>
       </c>
       <c r="AH7" s="272"/>
-      <c r="AI7" s="602"/>
+      <c r="AI7" s="580"/>
       <c r="AJ7" s="272"/>
-      <c r="AK7" s="602"/>
+      <c r="AK7" s="580"/>
       <c r="AL7" s="80" t="s">
         <v>515</v>
       </c>
       <c r="AM7" s="485"/>
-      <c r="AN7" s="588"/>
+      <c r="AN7" s="591"/>
       <c r="AP7" s="76" t="s">
         <v>489</v>
       </c>
@@ -7660,25 +7660,25 @@
         <f>SUM(G7:N9)</f>
         <v>16</v>
       </c>
-      <c r="F8" s="593"/>
-      <c r="G8" s="578">
-        <v>0</v>
-      </c>
-      <c r="H8" s="575" t="s">
+      <c r="F8" s="572"/>
+      <c r="G8" s="623">
+        <v>0</v>
+      </c>
+      <c r="H8" s="620" t="s">
         <v>105</v>
       </c>
       <c r="I8" s="524"/>
-      <c r="J8" s="575" t="s">
+      <c r="J8" s="620" t="s">
         <v>105</v>
       </c>
-      <c r="K8" s="581"/>
-      <c r="L8" s="611"/>
-      <c r="M8" s="594"/>
-      <c r="N8" s="614">
+      <c r="K8" s="626"/>
+      <c r="L8" s="582"/>
+      <c r="M8" s="595"/>
+      <c r="N8" s="587">
         <f>N5+N11</f>
         <v>15</v>
       </c>
-      <c r="O8" s="597"/>
+      <c r="O8" s="598"/>
       <c r="T8" s="103" t="s">
         <v>44</v>
       </c>
@@ -7696,14 +7696,14 @@
       <c r="AD8" s="16"/>
       <c r="AE8" s="272"/>
       <c r="AF8" s="272"/>
-      <c r="AG8" s="608"/>
+      <c r="AG8" s="581"/>
       <c r="AH8" s="272"/>
-      <c r="AI8" s="602"/>
+      <c r="AI8" s="580"/>
       <c r="AJ8" s="272"/>
       <c r="AK8" s="272"/>
       <c r="AL8" s="272"/>
       <c r="AM8" s="485"/>
-      <c r="AN8" s="588"/>
+      <c r="AN8" s="591"/>
     </row>
     <row r="9" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="245" t="s">
@@ -7718,17 +7718,17 @@
       <c r="D9" s="385" t="s">
         <v>286</v>
       </c>
-      <c r="F9" s="593"/>
-      <c r="G9" s="580"/>
-      <c r="H9" s="576"/>
+      <c r="F9" s="572"/>
+      <c r="G9" s="625"/>
+      <c r="H9" s="621"/>
       <c r="I9" s="526"/>
-      <c r="J9" s="576"/>
-      <c r="K9" s="582"/>
-      <c r="L9" s="612"/>
-      <c r="M9" s="595"/>
-      <c r="N9" s="615"/>
-      <c r="O9" s="598"/>
-      <c r="S9" s="609" t="s">
+      <c r="J9" s="621"/>
+      <c r="K9" s="627"/>
+      <c r="L9" s="583"/>
+      <c r="M9" s="596"/>
+      <c r="N9" s="588"/>
+      <c r="O9" s="599"/>
+      <c r="S9" s="584" t="s">
         <v>62</v>
       </c>
       <c r="T9" s="89"/>
@@ -7750,16 +7750,16 @@
       </c>
       <c r="AE9" s="272"/>
       <c r="AF9" s="272"/>
-      <c r="AG9" s="608"/>
+      <c r="AG9" s="581"/>
       <c r="AH9" s="272"/>
-      <c r="AI9" s="602"/>
+      <c r="AI9" s="580"/>
       <c r="AJ9" s="80"/>
-      <c r="AK9" s="602" t="s">
+      <c r="AK9" s="580" t="s">
         <v>256</v>
       </c>
       <c r="AL9" s="272"/>
       <c r="AM9" s="485"/>
-      <c r="AN9" s="588"/>
+      <c r="AN9" s="591"/>
       <c r="AP9" s="2" t="s">
         <v>527</v>
       </c>
@@ -7774,22 +7774,22 @@
       <c r="D10" s="142"/>
       <c r="E10" s="250">
         <f>Boat!S8</f>
-        <v>43</v>
-      </c>
-      <c r="F10" s="593"/>
+        <v>44</v>
+      </c>
+      <c r="F10" s="572"/>
       <c r="N10" s="475" t="s">
         <v>407</v>
       </c>
-      <c r="O10" s="626" t="s">
+      <c r="O10" s="574" t="s">
         <v>103</v>
       </c>
-      <c r="P10" s="599" t="s">
+      <c r="P10" s="600" t="s">
         <v>411</v>
       </c>
       <c r="R10" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="613"/>
+      <c r="S10" s="585"/>
       <c r="T10" s="89"/>
       <c r="U10" s="123" t="s">
         <v>177</v>
@@ -7819,16 +7819,16 @@
       <c r="AF10" s="251" t="s">
         <v>318</v>
       </c>
-      <c r="AG10" s="608"/>
+      <c r="AG10" s="581"/>
       <c r="AH10" s="80"/>
-      <c r="AI10" s="602"/>
+      <c r="AI10" s="580"/>
       <c r="AJ10" s="272"/>
-      <c r="AK10" s="602"/>
+      <c r="AK10" s="580"/>
       <c r="AL10" s="272"/>
       <c r="AM10" s="499" t="s">
         <v>325</v>
       </c>
-      <c r="AN10" s="588"/>
+      <c r="AN10" s="591"/>
       <c r="AO10" s="214" t="s">
         <v>95</v>
       </c>
@@ -7846,18 +7846,18 @@
       <c r="D11" s="175" t="s">
         <v>362</v>
       </c>
-      <c r="F11" s="593"/>
+      <c r="F11" s="572"/>
       <c r="M11" s="6"/>
       <c r="N11" s="117">
         <v>7</v>
       </c>
-      <c r="O11" s="627"/>
-      <c r="P11" s="600"/>
+      <c r="O11" s="575"/>
+      <c r="P11" s="601"/>
       <c r="Q11" s="65"/>
       <c r="R11" s="120" t="s">
         <v>222</v>
       </c>
-      <c r="S11" s="613"/>
+      <c r="S11" s="585"/>
       <c r="T11" s="102" t="s">
         <v>44</v>
       </c>
@@ -7881,14 +7881,14 @@
       <c r="AF11" s="272" t="s">
         <v>494</v>
       </c>
-      <c r="AG11" s="608"/>
+      <c r="AG11" s="581"/>
       <c r="AH11" s="272"/>
       <c r="AI11" s="70"/>
       <c r="AJ11" s="272"/>
       <c r="AK11" s="272"/>
       <c r="AL11" s="272"/>
       <c r="AM11" s="485"/>
-      <c r="AN11" s="588"/>
+      <c r="AN11" s="591"/>
       <c r="AP11" s="76" t="s">
         <v>502</v>
       </c>
@@ -7907,7 +7907,7 @@
       <c r="E12" s="237">
         <v>3</v>
       </c>
-      <c r="F12" s="593"/>
+      <c r="F12" s="572"/>
       <c r="G12" s="374" t="s">
         <v>411</v>
       </c>
@@ -7916,16 +7916,16 @@
       </c>
       <c r="I12" s="530"/>
       <c r="J12" s="530"/>
-      <c r="K12" s="631"/>
+      <c r="K12" s="579"/>
       <c r="L12" s="213"/>
       <c r="M12" s="213"/>
       <c r="N12" s="213"/>
-      <c r="O12" s="627"/>
-      <c r="P12" s="600"/>
+      <c r="O12" s="575"/>
+      <c r="P12" s="601"/>
       <c r="R12" s="122" t="s">
         <v>181</v>
       </c>
-      <c r="S12" s="610"/>
+      <c r="S12" s="586"/>
       <c r="T12" s="101" t="s">
         <v>44</v>
       </c>
@@ -7946,16 +7946,16 @@
       <c r="AC12" s="100" t="s">
         <v>499</v>
       </c>
-      <c r="AD12" s="616" t="s">
+      <c r="AD12" s="589" t="s">
         <v>245</v>
       </c>
       <c r="AE12" s="498" t="s">
         <v>244</v>
       </c>
-      <c r="AF12" s="608" t="s">
+      <c r="AF12" s="581" t="s">
         <v>231</v>
       </c>
-      <c r="AG12" s="608"/>
+      <c r="AG12" s="581"/>
       <c r="AH12" s="251" t="s">
         <v>264</v>
       </c>
@@ -7968,7 +7968,7 @@
       <c r="AM12" s="603" t="s">
         <v>254</v>
       </c>
-      <c r="AN12" s="588"/>
+      <c r="AN12" s="591"/>
       <c r="AO12" s="375" t="s">
         <v>97</v>
       </c>
@@ -7980,17 +7980,17 @@
       <c r="E13" s="505">
         <v>-3</v>
       </c>
-      <c r="F13" s="593"/>
+      <c r="F13" s="572"/>
       <c r="G13" s="530" t="s">
         <v>448</v>
       </c>
       <c r="H13" s="530"/>
       <c r="I13" s="530"/>
-      <c r="J13" s="631"/>
+      <c r="J13" s="579"/>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="627"/>
-      <c r="P13" s="601"/>
+      <c r="O13" s="575"/>
+      <c r="P13" s="602"/>
       <c r="T13" s="105" t="s">
         <v>44</v>
       </c>
@@ -8011,8 +8011,8 @@
         <v>519</v>
       </c>
       <c r="AC13" s="16"/>
-      <c r="AD13" s="616"/>
-      <c r="AF13" s="608"/>
+      <c r="AD13" s="589"/>
+      <c r="AF13" s="581"/>
       <c r="AG13" s="80"/>
       <c r="AH13" s="251" t="s">
         <v>314</v>
@@ -8024,7 +8024,7 @@
       <c r="AK13" s="272"/>
       <c r="AL13" s="272"/>
       <c r="AM13" s="603"/>
-      <c r="AN13" s="588"/>
+      <c r="AN13" s="591"/>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="507"/>
@@ -8032,18 +8032,18 @@
       <c r="C14" s="516"/>
       <c r="D14" s="509"/>
       <c r="E14" s="510"/>
-      <c r="F14" s="593"/>
+      <c r="F14" s="572"/>
       <c r="G14" s="530" t="s">
         <v>447</v>
       </c>
       <c r="H14" s="530"/>
       <c r="I14" s="530"/>
-      <c r="J14" s="631"/>
+      <c r="J14" s="579"/>
       <c r="K14" s="2">
         <v>12</v>
       </c>
       <c r="N14" s="6"/>
-      <c r="O14" s="627"/>
+      <c r="O14" s="575"/>
       <c r="Q14" s="61" t="s">
         <v>562</v>
       </c>
@@ -8064,9 +8064,9 @@
       <c r="AA14" s="325"/>
       <c r="AB14" s="219"/>
       <c r="AC14" s="16"/>
-      <c r="AD14" s="616"/>
+      <c r="AD14" s="589"/>
       <c r="AE14" s="272"/>
-      <c r="AF14" s="608"/>
+      <c r="AF14" s="581"/>
       <c r="AG14" s="272"/>
       <c r="AH14" s="272"/>
       <c r="AI14" s="70"/>
@@ -8074,7 +8074,7 @@
       <c r="AK14" s="272"/>
       <c r="AL14" s="272"/>
       <c r="AM14" s="603"/>
-      <c r="AN14" s="588"/>
+      <c r="AN14" s="591"/>
     </row>
     <row r="15" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="506" t="s">
@@ -8083,8 +8083,8 @@
       <c r="C15" s="524" t="s">
         <v>382</v>
       </c>
-      <c r="F15" s="593"/>
-      <c r="O15" s="627"/>
+      <c r="F15" s="572"/>
+      <c r="O15" s="575"/>
       <c r="R15" s="99" t="s">
         <v>44</v>
       </c>
@@ -8106,8 +8106,8 @@
       <c r="AC15" s="76" t="s">
         <v>497</v>
       </c>
-      <c r="AD15" s="616"/>
-      <c r="AF15" s="608"/>
+      <c r="AD15" s="589"/>
+      <c r="AF15" s="581"/>
       <c r="AG15" s="80"/>
       <c r="AH15" s="251" t="s">
         <v>466</v>
@@ -8121,7 +8121,7 @@
       <c r="AK15" s="272"/>
       <c r="AL15" s="272"/>
       <c r="AM15" s="603"/>
-      <c r="AN15" s="588"/>
+      <c r="AN15" s="591"/>
       <c r="AP15" s="76" t="s">
         <v>74</v>
       </c>
@@ -8143,13 +8143,13 @@
       <c r="E16" s="237">
         <v>1</v>
       </c>
-      <c r="F16" s="593"/>
+      <c r="F16" s="572"/>
       <c r="G16" s="374" t="s">
         <v>506</v>
       </c>
       <c r="I16" s="20"/>
       <c r="J16" s="20"/>
-      <c r="O16" s="627"/>
+      <c r="O16" s="575"/>
       <c r="R16" s="492" t="s">
         <v>185</v>
       </c>
@@ -8181,18 +8181,18 @@
       <c r="AM16" s="485" t="s">
         <v>324</v>
       </c>
-      <c r="AN16" s="588"/>
+      <c r="AN16" s="591"/>
       <c r="AP16" s="76" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="80"/>
-      <c r="F17" s="593"/>
+      <c r="F17" s="572"/>
       <c r="I17" s="20"/>
       <c r="J17" s="20"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="627"/>
+      <c r="O17" s="575"/>
       <c r="Q17" s="21" t="s">
         <v>560</v>
       </c>
@@ -8237,7 +8237,7 @@
       <c r="AK17" s="272"/>
       <c r="AL17" s="80"/>
       <c r="AM17" s="485"/>
-      <c r="AN17" s="588"/>
+      <c r="AN17" s="591"/>
       <c r="AO17" s="214" t="s">
         <v>516</v>
       </c>
@@ -8261,21 +8261,21 @@
       <c r="E18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="F18" s="593"/>
+      <c r="F18" s="572"/>
       <c r="G18" s="374" t="s">
         <v>557</v>
       </c>
       <c r="I18" s="20"/>
       <c r="J18" s="20"/>
-      <c r="O18" s="627"/>
+      <c r="O18" s="575"/>
       <c r="Q18" s="112"/>
-      <c r="R18" s="621" t="s">
+      <c r="R18" s="567" t="s">
         <v>565</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
       </c>
-      <c r="U18" s="566" t="s">
+      <c r="U18" s="611" t="s">
         <v>44</v>
       </c>
       <c r="V18" s="120"/>
@@ -8296,7 +8296,7 @@
       <c r="AC18" s="16"/>
       <c r="AD18" s="16"/>
       <c r="AE18" s="272"/>
-      <c r="AF18" s="602" t="s">
+      <c r="AF18" s="580" t="s">
         <v>493</v>
       </c>
       <c r="AG18" s="272"/>
@@ -8308,19 +8308,19 @@
       <c r="AK18" s="272"/>
       <c r="AL18" s="80"/>
       <c r="AM18" s="485"/>
-      <c r="AN18" s="588"/>
+      <c r="AN18" s="591"/>
       <c r="AP18" s="76" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="593"/>
-      <c r="O19" s="627"/>
-      <c r="R19" s="622"/>
+      <c r="F19" s="572"/>
+      <c r="O19" s="575"/>
+      <c r="R19" s="568"/>
       <c r="S19" s="30" t="s">
         <v>563</v>
       </c>
-      <c r="U19" s="567"/>
+      <c r="U19" s="612"/>
       <c r="V19" s="146"/>
       <c r="W19" s="146"/>
       <c r="X19" s="488" t="s">
@@ -8335,7 +8335,7 @@
       <c r="AC19" s="16"/>
       <c r="AD19" s="16"/>
       <c r="AE19" s="272"/>
-      <c r="AF19" s="602"/>
+      <c r="AF19" s="580"/>
       <c r="AG19" s="272"/>
       <c r="AH19" s="272"/>
       <c r="AI19" s="70"/>
@@ -8345,7 +8345,7 @@
       </c>
       <c r="AL19" s="80"/>
       <c r="AM19" s="485"/>
-      <c r="AN19" s="588"/>
+      <c r="AN19" s="591"/>
       <c r="AP19" s="76" t="s">
         <v>486</v>
       </c>
@@ -8366,18 +8366,18 @@
       <c r="E20" s="494">
         <v>-1</v>
       </c>
-      <c r="F20" s="593"/>
+      <c r="F20" s="572"/>
       <c r="G20" s="374" t="s">
         <v>509</v>
       </c>
-      <c r="O20" s="627"/>
-      <c r="Q20" s="629" t="s">
+      <c r="O20" s="575"/>
+      <c r="Q20" s="577" t="s">
         <v>48</v>
       </c>
       <c r="T20" s="461" t="s">
         <v>44</v>
       </c>
-      <c r="U20" s="568"/>
+      <c r="U20" s="613"/>
       <c r="W20" s="462"/>
       <c r="X20" s="489" t="s">
         <v>175</v>
@@ -8407,7 +8407,7 @@
       <c r="AM20" s="427" t="s">
         <v>254</v>
       </c>
-      <c r="AN20" s="588"/>
+      <c r="AN20" s="591"/>
       <c r="AO20" s="375" t="s">
         <v>478</v>
       </c>
@@ -8431,12 +8431,12 @@
       <c r="E21" s="281">
         <v>1</v>
       </c>
-      <c r="F21" s="593"/>
-      <c r="O21" s="627"/>
-      <c r="Q21" s="630"/>
+      <c r="F21" s="572"/>
+      <c r="O21" s="575"/>
+      <c r="Q21" s="578"/>
       <c r="T21" s="479"/>
       <c r="U21" s="14"/>
-      <c r="V21" s="563"/>
+      <c r="V21" s="608"/>
       <c r="W21" s="483" t="s">
         <v>176</v>
       </c>
@@ -8474,14 +8474,14 @@
       <c r="AM21" s="485" t="s">
         <v>575</v>
       </c>
-      <c r="AN21" s="588"/>
+      <c r="AN21" s="591"/>
     </row>
     <row r="22" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F22" s="593"/>
+      <c r="F22" s="572"/>
       <c r="G22" s="374" t="s">
         <v>507</v>
       </c>
-      <c r="O22" s="627"/>
+      <c r="O22" s="575"/>
       <c r="R22" s="491" t="s">
         <v>44</v>
       </c>
@@ -8489,7 +8489,7 @@
         <v>44</v>
       </c>
       <c r="U22" s="15"/>
-      <c r="V22" s="564"/>
+      <c r="V22" s="609"/>
       <c r="W22" s="483" t="s">
         <v>176</v>
       </c>
@@ -8507,7 +8507,7 @@
       <c r="AG22" s="6"/>
       <c r="AH22" s="6"/>
       <c r="AI22" s="6"/>
-      <c r="AJ22" s="602" t="s">
+      <c r="AJ22" s="580" t="s">
         <v>490</v>
       </c>
       <c r="AK22" s="272"/>
@@ -8515,7 +8515,7 @@
         <v>496</v>
       </c>
       <c r="AM22" s="318"/>
-      <c r="AN22" s="588"/>
+      <c r="AN22" s="591"/>
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="244" t="s">
@@ -8533,16 +8533,16 @@
       <c r="E23" s="238">
         <v>1</v>
       </c>
-      <c r="F23" s="593"/>
-      <c r="O23" s="627"/>
-      <c r="Q23" s="629" t="s">
+      <c r="F23" s="572"/>
+      <c r="O23" s="575"/>
+      <c r="Q23" s="577" t="s">
         <v>145</v>
       </c>
       <c r="T23" s="17"/>
       <c r="U23" s="477" t="s">
         <v>44</v>
       </c>
-      <c r="V23" s="564"/>
+      <c r="V23" s="609"/>
       <c r="W23" s="148"/>
       <c r="X23" s="486" t="s">
         <v>189</v>
@@ -8558,13 +8558,13 @@
       <c r="AG23" s="6"/>
       <c r="AH23" s="6"/>
       <c r="AI23" s="6"/>
-      <c r="AJ23" s="602"/>
+      <c r="AJ23" s="580"/>
       <c r="AK23" s="272"/>
       <c r="AL23" s="80" t="s">
         <v>526</v>
       </c>
       <c r="AM23" s="318"/>
-      <c r="AN23" s="588"/>
+      <c r="AN23" s="591"/>
     </row>
     <row r="24" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="497" t="s">
@@ -8582,17 +8582,17 @@
       <c r="E24" s="493">
         <v>1</v>
       </c>
-      <c r="F24" s="593"/>
+      <c r="F24" s="572"/>
       <c r="G24" s="61" t="s">
         <v>508</v>
       </c>
-      <c r="O24" s="627"/>
-      <c r="Q24" s="630"/>
+      <c r="O24" s="575"/>
+      <c r="Q24" s="578"/>
       <c r="T24" s="17"/>
       <c r="U24" s="240" t="s">
         <v>44</v>
       </c>
-      <c r="V24" s="564"/>
+      <c r="V24" s="609"/>
       <c r="W24" s="148"/>
       <c r="X24" s="486" t="s">
         <v>186</v>
@@ -8616,11 +8616,11 @@
         <v>481</v>
       </c>
       <c r="AM24" s="318"/>
-      <c r="AN24" s="588"/>
+      <c r="AN24" s="591"/>
     </row>
     <row r="25" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F25" s="593"/>
-      <c r="O25" s="627"/>
+      <c r="F25" s="572"/>
+      <c r="O25" s="575"/>
       <c r="P25" s="214" t="s">
         <v>285</v>
       </c>
@@ -8633,7 +8633,7 @@
       <c r="U25" s="454" t="s">
         <v>44</v>
       </c>
-      <c r="V25" s="565"/>
+      <c r="V25" s="610"/>
       <c r="W25" s="148"/>
       <c r="X25" s="486" t="s">
         <v>190</v>
@@ -8655,7 +8655,7 @@
       <c r="AK25" s="142"/>
       <c r="AL25" s="6"/>
       <c r="AM25" s="318"/>
-      <c r="AN25" s="588"/>
+      <c r="AN25" s="591"/>
     </row>
     <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="244" t="s">
@@ -8673,16 +8673,16 @@
       <c r="E26" s="424">
         <v>1</v>
       </c>
-      <c r="F26" s="593"/>
+      <c r="F26" s="572"/>
       <c r="G26" s="374" t="s">
         <v>505</v>
       </c>
-      <c r="O26" s="627"/>
-      <c r="P26" s="590" t="s">
+      <c r="O26" s="575"/>
+      <c r="P26" s="593" t="s">
         <v>551</v>
       </c>
-      <c r="Q26" s="591"/>
-      <c r="R26" s="623" t="s">
+      <c r="Q26" s="594"/>
+      <c r="R26" s="569" t="s">
         <v>564</v>
       </c>
       <c r="T26" s="183"/>
@@ -8721,7 +8721,7 @@
       <c r="AM26" s="499" t="s">
         <v>474</v>
       </c>
-      <c r="AN26" s="588"/>
+      <c r="AN26" s="591"/>
     </row>
     <row r="27" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="21" t="s">
@@ -8733,12 +8733,12 @@
       <c r="E27" s="281" t="s">
         <v>44</v>
       </c>
-      <c r="F27" s="625"/>
+      <c r="F27" s="573"/>
       <c r="G27" s="61" t="s">
         <v>574</v>
       </c>
-      <c r="O27" s="628"/>
-      <c r="R27" s="624"/>
+      <c r="O27" s="576"/>
+      <c r="R27" s="570"/>
       <c r="S27" s="478" t="s">
         <v>54</v>
       </c>
@@ -8768,32 +8768,26 @@
       <c r="AM27" s="427" t="s">
         <v>326</v>
       </c>
-      <c r="AN27" s="589"/>
+      <c r="AN27" s="592"/>
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="R26:R27"/>
-    <mergeCell ref="F2:F27"/>
-    <mergeCell ref="O10:O27"/>
-    <mergeCell ref="Q20:Q21"/>
-    <mergeCell ref="Q23:Q24"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="AI6:AI10"/>
-    <mergeCell ref="AF12:AF15"/>
-    <mergeCell ref="AG7:AG12"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="S9:S12"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="AD12:AD15"/>
-    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="V21:V25"/>
+    <mergeCell ref="U18:U20"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="G5:L6"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B4:B5"/>
     <mergeCell ref="AN1:AN27"/>
     <mergeCell ref="P26:Q26"/>
     <mergeCell ref="Q2:Q3"/>
@@ -8810,22 +8804,28 @@
     <mergeCell ref="AD3:AD4"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="R2:R3"/>
-    <mergeCell ref="V21:V25"/>
-    <mergeCell ref="U18:U20"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="G5:L6"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="AI6:AI10"/>
+    <mergeCell ref="AF12:AF15"/>
+    <mergeCell ref="AG7:AG12"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="S9:S12"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="AD12:AD15"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="R26:R27"/>
+    <mergeCell ref="F2:F27"/>
+    <mergeCell ref="O10:O27"/>
+    <mergeCell ref="Q20:Q21"/>
+    <mergeCell ref="Q23:Q24"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="H12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8835,8 +8835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AN37"/>
   <sheetViews>
-    <sheetView topLeftCell="O5" workbookViewId="0">
-      <selection activeCell="AG25" sqref="AG25"/>
+    <sheetView tabSelected="1" topLeftCell="J4" workbookViewId="0">
+      <selection activeCell="AF20" sqref="AF20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8926,13 +8926,13 @@
       <c r="T1" s="559" t="s">
         <v>236</v>
       </c>
-      <c r="U1" s="647" t="s">
+      <c r="U1" s="636" t="s">
         <v>237</v>
       </c>
-      <c r="V1" s="649" t="s">
+      <c r="V1" s="638" t="s">
         <v>459</v>
       </c>
-      <c r="W1" s="650"/>
+      <c r="W1" s="639"/>
       <c r="X1" s="324">
         <f>68-(S8+W3+V3+Q3)</f>
         <v>0</v>
@@ -8948,40 +8948,40 @@
       <c r="AB1" s="320" t="s">
         <v>44</v>
       </c>
-      <c r="AC1" s="651" t="s">
+      <c r="AC1" s="640" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="652"/>
-      <c r="AE1" s="653"/>
-      <c r="AF1" s="654" t="s">
+      <c r="AD1" s="641"/>
+      <c r="AE1" s="642"/>
+      <c r="AF1" s="643" t="s">
         <v>298</v>
       </c>
-      <c r="AG1" s="655"/>
-      <c r="AH1" s="656"/>
-      <c r="AI1" s="643" t="s">
+      <c r="AG1" s="644"/>
+      <c r="AH1" s="645"/>
+      <c r="AI1" s="632" t="s">
         <v>462</v>
       </c>
-      <c r="AJ1" s="644"/>
-      <c r="AK1" s="645"/>
+      <c r="AJ1" s="633"/>
+      <c r="AK1" s="634"/>
       <c r="AN1" s="112"/>
     </row>
     <row r="2" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F2" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="J2" s="635">
+      <c r="J2" s="646">
         <f>SUM(J5:J30)</f>
         <v>0</v>
       </c>
-      <c r="K2" s="637">
+      <c r="K2" s="648">
         <f>SUM(K4:K29)</f>
+        <v>3</v>
+      </c>
+      <c r="L2" s="650">
+        <f>SUM(L4:L29)</f>
         <v>4</v>
       </c>
-      <c r="L2" s="639">
-        <f>SUM(L4:L29)</f>
-        <v>5</v>
-      </c>
-      <c r="M2" s="614">
+      <c r="M2" s="587">
         <f>SUM(K30:K37)* (-1)</f>
         <v>1</v>
       </c>
@@ -9000,11 +9000,11 @@
       <c r="R2" s="61" t="s">
         <v>221</v>
       </c>
-      <c r="S2" s="641" t="s">
+      <c r="S2" s="652" t="s">
         <v>239</v>
       </c>
-      <c r="T2" s="646"/>
-      <c r="U2" s="648"/>
+      <c r="T2" s="635"/>
+      <c r="U2" s="637"/>
       <c r="V2" s="61" t="s">
         <v>456</v>
       </c>
@@ -9064,10 +9064,10 @@
       </c>
     </row>
     <row r="3" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J3" s="636"/>
-      <c r="K3" s="638"/>
-      <c r="L3" s="640"/>
-      <c r="M3" s="615"/>
+      <c r="J3" s="647"/>
+      <c r="K3" s="649"/>
+      <c r="L3" s="651"/>
+      <c r="M3" s="588"/>
       <c r="N3" s="177">
         <f>(J2+K2)-W3</f>
         <v>0</v>
@@ -9081,9 +9081,9 @@
       </c>
       <c r="R3" s="159">
         <f>SUM(R4:R29)</f>
-        <v>43</v>
-      </c>
-      <c r="S3" s="642"/>
+        <v>44</v>
+      </c>
+      <c r="S3" s="653"/>
       <c r="T3" s="560"/>
       <c r="U3" s="331">
         <f>R3+V3+W3+Q3</f>
@@ -9095,7 +9095,7 @@
       </c>
       <c r="W3" s="187">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X3" s="59">
         <f t="shared" si="0"/>
@@ -9103,15 +9103,15 @@
       </c>
       <c r="Y3" s="66">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Z3" s="66">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AA3" s="66">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AB3" s="66">
         <f t="shared" ref="AB3:AK3" si="1">SUM(AB4:AB29)</f>
@@ -9119,7 +9119,7 @@
       </c>
       <c r="AC3" s="66">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AD3" s="66">
         <f t="shared" si="1"/>
@@ -9131,7 +9131,7 @@
       </c>
       <c r="AF3" s="66">
         <f>SUM(AF4:AF29)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AG3" s="412">
         <f t="shared" si="1"/>
@@ -9143,15 +9143,15 @@
       </c>
       <c r="AI3" s="100">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AJ3" s="329">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AK3" s="330">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AN3" s="112"/>
     </row>
@@ -9185,7 +9185,7 @@
         <f>AA4</f>
         <v>0</v>
       </c>
-      <c r="M4" s="632" t="s">
+      <c r="M4" s="654" t="s">
         <v>200</v>
       </c>
       <c r="N4" s="20"/>
@@ -9264,7 +9264,7 @@
         <f>AA5</f>
         <v>0</v>
       </c>
-      <c r="M5" s="633"/>
+      <c r="M5" s="655"/>
       <c r="N5" s="20"/>
       <c r="O5" s="2" t="s">
         <v>347</v>
@@ -9352,7 +9352,7 @@
         <f>AA6</f>
         <v>0</v>
       </c>
-      <c r="M6" s="633"/>
+      <c r="M6" s="655"/>
       <c r="N6" s="19" t="s">
         <v>342</v>
       </c>
@@ -9442,7 +9442,7 @@
         <f t="shared" ref="L7:L37" si="10">AA7</f>
         <v>0</v>
       </c>
-      <c r="M7" s="633"/>
+      <c r="M7" s="655"/>
       <c r="N7" s="20"/>
       <c r="O7" s="2" t="s">
         <v>342</v>
@@ -9550,7 +9550,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M8" s="633"/>
+      <c r="M8" s="655"/>
       <c r="N8" s="21" t="s">
         <v>238</v>
       </c>
@@ -9568,7 +9568,7 @@
       </c>
       <c r="S8" s="340">
         <f>R3</f>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="T8" s="17"/>
       <c r="U8" s="348"/>
@@ -9636,7 +9636,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M9" s="633"/>
+      <c r="M9" s="655"/>
       <c r="N9" s="21" t="s">
         <v>342</v>
       </c>
@@ -9736,7 +9736,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M10" s="633"/>
+      <c r="M10" s="655"/>
       <c r="N10" s="20"/>
       <c r="O10" s="2" t="s">
         <v>347</v>
@@ -9815,7 +9815,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M11" s="633"/>
+      <c r="M11" s="655"/>
       <c r="N11" s="21" t="s">
         <v>342</v>
       </c>
@@ -9877,7 +9877,7 @@
       <c r="AN11" s="112"/>
     </row>
     <row r="12" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="578" t="s">
+      <c r="A12" s="623" t="s">
         <v>55</v>
       </c>
       <c r="B12" s="30">
@@ -9886,7 +9886,7 @@
       <c r="C12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="629" t="s">
+      <c r="E12" s="577" t="s">
         <v>57</v>
       </c>
       <c r="G12" s="277">
@@ -9906,7 +9906,7 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="M12" s="633"/>
+      <c r="M12" s="655"/>
       <c r="N12" s="21" t="s">
         <v>342</v>
       </c>
@@ -9980,14 +9980,14 @@
       </c>
     </row>
     <row r="13" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="580"/>
+      <c r="A13" s="625"/>
       <c r="B13" s="153">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="630"/>
+      <c r="E13" s="578"/>
       <c r="F13" s="177">
         <v>0</v>
       </c>
@@ -10008,7 +10008,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M13" s="633"/>
+      <c r="M13" s="655"/>
       <c r="N13" s="21" t="s">
         <v>342</v>
       </c>
@@ -10083,7 +10083,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M14" s="633"/>
+      <c r="M14" s="655"/>
       <c r="N14" s="20"/>
       <c r="O14" s="210" t="s">
         <v>346</v>
@@ -10166,7 +10166,7 @@
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="M15" s="633"/>
+      <c r="M15" s="655"/>
       <c r="N15" s="20"/>
       <c r="O15" s="210" t="s">
         <v>346</v>
@@ -10247,13 +10247,13 @@
       <c r="I16" s="434"/>
       <c r="J16" s="363"/>
       <c r="K16" s="107">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L16" s="311">
         <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="M16" s="633"/>
+        <v>0</v>
+      </c>
+      <c r="M16" s="655"/>
       <c r="N16" s="21" t="s">
         <v>342</v>
       </c>
@@ -10265,7 +10265,7 @@
       </c>
       <c r="Q16" s="164"/>
       <c r="R16" s="157">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S16" s="338">
         <v>-3</v>
@@ -10275,46 +10275,48 @@
       <c r="V16" s="345"/>
       <c r="W16" s="190">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X16" s="314"/>
       <c r="Y16" s="117">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z16" s="308">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AA16" s="308">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB16" s="308">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AC16" s="312">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD16" s="318"/>
       <c r="AE16" s="314"/>
       <c r="AF16" s="314">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="AG16" s="373"/>
+        <v>0</v>
+      </c>
+      <c r="AG16" s="373">
+        <v>0</v>
+      </c>
       <c r="AH16" s="158"/>
       <c r="AI16" s="326">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ16" s="327">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK16" s="328">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL16" s="6" t="s">
         <v>235</v>
@@ -10340,7 +10342,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M17" s="633"/>
+      <c r="M17" s="655"/>
       <c r="N17" s="20"/>
       <c r="O17" s="2" t="s">
         <v>348</v>
@@ -10423,7 +10425,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M18" s="633"/>
+      <c r="M18" s="655"/>
       <c r="N18" s="21" t="s">
         <v>342</v>
       </c>
@@ -10510,7 +10512,7 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M19" s="633"/>
+      <c r="M19" s="655"/>
       <c r="N19" s="20"/>
       <c r="O19" s="2" t="s">
         <v>341</v>
@@ -10599,11 +10601,11 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="M20" s="634"/>
+      <c r="M20" s="656"/>
       <c r="N20" s="529" t="s">
         <v>342</v>
       </c>
-      <c r="O20" s="631"/>
+      <c r="O20" s="579"/>
       <c r="P20" s="334" t="s">
         <v>86</v>
       </c>
@@ -10844,7 +10846,7 @@
       <c r="AN22" s="112"/>
     </row>
     <row r="23" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E23" s="585" t="s">
+      <c r="E23" s="630" t="s">
         <v>294</v>
       </c>
       <c r="F23" s="185">
@@ -10930,7 +10932,7 @@
       <c r="C24" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E24" s="586"/>
+      <c r="E24" s="631"/>
       <c r="F24" s="177"/>
       <c r="I24" s="431" t="s">
         <v>301</v>
@@ -10948,7 +10950,7 @@
       <c r="N24" s="529" t="s">
         <v>342</v>
       </c>
-      <c r="O24" s="631"/>
+      <c r="O24" s="579"/>
       <c r="P24" s="334" t="s">
         <v>254</v>
       </c>
@@ -12018,23 +12020,23 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="M4:M20"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="S2:S3"/>
     <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="T1:T3"/>
     <mergeCell ref="U1:U2"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="AC1:AE1"/>
     <mergeCell ref="AF1:AH1"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="M4:M20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12071,12 +12073,12 @@
       <c r="B1" s="529" t="s">
         <v>317</v>
       </c>
-      <c r="C1" s="631"/>
+      <c r="C1" s="579"/>
       <c r="D1" s="214"/>
       <c r="J1" s="529" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="631"/>
+      <c r="K1" s="579"/>
       <c r="L1" s="205" t="s">
         <v>337</v>
       </c>
@@ -12467,7 +12469,7 @@
       <c r="V1" s="529" t="s">
         <v>71</v>
       </c>
-      <c r="W1" s="631"/>
+      <c r="W1" s="579"/>
       <c r="X1" s="62" t="s">
         <v>102</v>
       </c>
@@ -12486,7 +12488,7 @@
       <c r="AC1" s="116" t="s">
         <v>191</v>
       </c>
-      <c r="AD1" s="677" t="s">
+      <c r="AD1" s="670" t="s">
         <v>213</v>
       </c>
       <c r="AE1" s="116" t="s">
@@ -12503,10 +12505,10 @@
       <c r="E2" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="708" t="s">
+      <c r="F2" s="669" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="665" t="s">
+      <c r="G2" s="697" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -12534,10 +12536,10 @@
       <c r="U2" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="V2" s="649" t="s">
+      <c r="V2" s="638" t="s">
         <v>121</v>
       </c>
-      <c r="W2" s="650"/>
+      <c r="W2" s="639"/>
       <c r="X2" s="64" t="s">
         <v>110</v>
       </c>
@@ -12556,7 +12558,7 @@
       <c r="AC2" s="117" t="s">
         <v>99</v>
       </c>
-      <c r="AD2" s="678"/>
+      <c r="AD2" s="671"/>
       <c r="AE2" s="64" t="s">
         <v>99</v>
       </c>
@@ -12575,8 +12577,8 @@
       <c r="E3" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="582"/>
-      <c r="G3" s="666"/>
+      <c r="F3" s="627"/>
+      <c r="G3" s="698"/>
       <c r="H3" s="40" t="s">
         <v>81</v>
       </c>
@@ -12587,13 +12589,13 @@
         <v>82</v>
       </c>
       <c r="N3" s="44"/>
-      <c r="O3" s="675" t="s">
+      <c r="O3" s="707" t="s">
         <v>44</v>
       </c>
-      <c r="P3" s="696" t="s">
+      <c r="P3" s="689" t="s">
         <v>219</v>
       </c>
-      <c r="Q3" s="697"/>
+      <c r="Q3" s="690"/>
       <c r="S3" s="57" t="s">
         <v>220</v>
       </c>
@@ -12603,15 +12605,15 @@
       <c r="W3" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="AD3" s="678"/>
+      <c r="AD3" s="671"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G4" s="666"/>
+      <c r="G4" s="698"/>
       <c r="H4" s="6"/>
       <c r="L4" s="660" t="s">
         <v>83</v>
       </c>
-      <c r="O4" s="676"/>
+      <c r="O4" s="708"/>
       <c r="T4" s="55" t="s">
         <v>98</v>
       </c>
@@ -12625,8 +12627,8 @@
         <v>195</v>
       </c>
       <c r="Z4" s="530"/>
-      <c r="AA4" s="631"/>
-      <c r="AD4" s="678"/>
+      <c r="AA4" s="579"/>
+      <c r="AD4" s="671"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="52" t="s">
@@ -12641,21 +12643,21 @@
       <c r="F5" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="666"/>
+      <c r="G5" s="698"/>
       <c r="H5" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="683" t="s">
+      <c r="K5" s="676" t="s">
         <v>217</v>
       </c>
-      <c r="L5" s="698"/>
+      <c r="L5" s="691"/>
       <c r="M5" s="2" t="s">
         <v>215</v>
       </c>
       <c r="N5" s="61" t="s">
         <v>214</v>
       </c>
-      <c r="O5" s="676"/>
+      <c r="O5" s="708"/>
       <c r="P5" s="108" t="s">
         <v>216</v>
       </c>
@@ -12671,11 +12673,11 @@
       <c r="U5" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="Y5" s="686" t="s">
+      <c r="Y5" s="679" t="s">
         <v>287</v>
       </c>
-      <c r="Z5" s="687"/>
-      <c r="AD5" s="678"/>
+      <c r="Z5" s="680"/>
+      <c r="AD5" s="671"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="109"/>
@@ -12685,16 +12687,16 @@
       <c r="E6" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="666"/>
+      <c r="G6" s="698"/>
       <c r="H6" s="46" t="s">
         <v>81</v>
       </c>
       <c r="I6" s="23">
         <v>15</v>
       </c>
-      <c r="K6" s="684"/>
-      <c r="L6" s="698"/>
-      <c r="O6" s="676"/>
+      <c r="K6" s="677"/>
+      <c r="L6" s="691"/>
+      <c r="O6" s="708"/>
       <c r="S6" s="104" t="s">
         <v>20</v>
       </c>
@@ -12707,20 +12709,20 @@
       <c r="V6" s="21">
         <v>-1</v>
       </c>
-      <c r="AD6" s="678"/>
+      <c r="AD6" s="671"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="110"/>
-      <c r="G7" s="666"/>
+      <c r="G7" s="698"/>
       <c r="H7" s="6"/>
-      <c r="K7" s="684"/>
-      <c r="L7" s="698"/>
+      <c r="K7" s="677"/>
+      <c r="L7" s="691"/>
       <c r="N7" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="O7" s="676"/>
+      <c r="O7" s="708"/>
       <c r="P7" s="73"/>
-      <c r="AD7" s="678"/>
+      <c r="AD7" s="671"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="130"/>
@@ -12733,7 +12735,7 @@
       <c r="F8" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="666"/>
+      <c r="G8" s="698"/>
       <c r="H8" s="50" t="s">
         <v>76</v>
       </c>
@@ -12743,41 +12745,41 @@
       <c r="J8" s="111">
         <v>115</v>
       </c>
-      <c r="K8" s="684"/>
-      <c r="L8" s="698"/>
-      <c r="O8" s="676"/>
+      <c r="K8" s="677"/>
+      <c r="L8" s="691"/>
+      <c r="O8" s="708"/>
       <c r="P8" s="49"/>
-      <c r="S8" s="680" t="s">
+      <c r="S8" s="673" t="s">
         <v>212</v>
       </c>
-      <c r="T8" s="681"/>
-      <c r="U8" s="681"/>
-      <c r="V8" s="681"/>
-      <c r="W8" s="681"/>
-      <c r="X8" s="681"/>
-      <c r="Y8" s="681"/>
-      <c r="Z8" s="681"/>
-      <c r="AA8" s="681"/>
-      <c r="AB8" s="681"/>
-      <c r="AC8" s="682"/>
-      <c r="AD8" s="678"/>
+      <c r="T8" s="674"/>
+      <c r="U8" s="674"/>
+      <c r="V8" s="674"/>
+      <c r="W8" s="674"/>
+      <c r="X8" s="674"/>
+      <c r="Y8" s="674"/>
+      <c r="Z8" s="674"/>
+      <c r="AA8" s="674"/>
+      <c r="AB8" s="674"/>
+      <c r="AC8" s="675"/>
+      <c r="AD8" s="671"/>
     </row>
     <row r="9" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="702"/>
-      <c r="G9" s="666"/>
+      <c r="C9" s="663"/>
+      <c r="G9" s="698"/>
       <c r="H9" s="6"/>
-      <c r="K9" s="684"/>
-      <c r="L9" s="669" t="s">
+      <c r="K9" s="677"/>
+      <c r="L9" s="701" t="s">
         <v>218</v>
       </c>
-      <c r="M9" s="670"/>
-      <c r="N9" s="671"/>
-      <c r="O9" s="676"/>
+      <c r="M9" s="702"/>
+      <c r="N9" s="703"/>
+      <c r="O9" s="708"/>
       <c r="P9" s="75"/>
-      <c r="AD9" s="678"/>
+      <c r="AD9" s="671"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="703"/>
+      <c r="C10" s="664"/>
       <c r="D10" s="23"/>
       <c r="E10" s="45" t="s">
         <v>88</v>
@@ -12785,7 +12787,7 @@
       <c r="F10" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="G10" s="666"/>
+      <c r="G10" s="698"/>
       <c r="H10" s="51"/>
       <c r="I10" s="21" t="s">
         <v>81</v>
@@ -12793,33 +12795,33 @@
       <c r="J10" s="3">
         <v>15</v>
       </c>
-      <c r="K10" s="684"/>
-      <c r="M10" s="705" t="s">
+      <c r="K10" s="677"/>
+      <c r="M10" s="666" t="s">
         <v>90</v>
       </c>
-      <c r="N10" s="706"/>
-      <c r="O10" s="706"/>
-      <c r="P10" s="706"/>
-      <c r="Q10" s="706"/>
-      <c r="R10" s="706"/>
-      <c r="S10" s="706"/>
-      <c r="T10" s="706"/>
-      <c r="U10" s="706"/>
-      <c r="V10" s="706"/>
-      <c r="W10" s="706"/>
-      <c r="X10" s="706"/>
-      <c r="Y10" s="706"/>
-      <c r="Z10" s="706"/>
-      <c r="AA10" s="706"/>
-      <c r="AB10" s="706"/>
-      <c r="AC10" s="707"/>
-      <c r="AD10" s="678"/>
+      <c r="N10" s="667"/>
+      <c r="O10" s="667"/>
+      <c r="P10" s="667"/>
+      <c r="Q10" s="667"/>
+      <c r="R10" s="667"/>
+      <c r="S10" s="667"/>
+      <c r="T10" s="667"/>
+      <c r="U10" s="667"/>
+      <c r="V10" s="667"/>
+      <c r="W10" s="667"/>
+      <c r="X10" s="667"/>
+      <c r="Y10" s="667"/>
+      <c r="Z10" s="667"/>
+      <c r="AA10" s="667"/>
+      <c r="AB10" s="667"/>
+      <c r="AC10" s="668"/>
+      <c r="AD10" s="671"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="704"/>
-      <c r="G11" s="666"/>
+      <c r="C11" s="665"/>
+      <c r="G11" s="698"/>
       <c r="H11" s="6"/>
-      <c r="K11" s="684"/>
+      <c r="K11" s="677"/>
       <c r="R11" s="52" t="s">
         <v>44</v>
       </c>
@@ -12827,17 +12829,17 @@
       <c r="Y11" s="68" t="s">
         <v>121</v>
       </c>
-      <c r="Z11" s="694" t="s">
+      <c r="Z11" s="687" t="s">
         <v>121</v>
       </c>
-      <c r="AA11" s="695"/>
+      <c r="AA11" s="688"/>
       <c r="AB11" s="52" t="s">
         <v>44</v>
       </c>
       <c r="AC11" s="118" t="s">
         <v>121</v>
       </c>
-      <c r="AD11" s="678"/>
+      <c r="AD11" s="671"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="129"/>
@@ -12850,7 +12852,7 @@
       <c r="F12" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="G12" s="666"/>
+      <c r="G12" s="698"/>
       <c r="H12" s="128"/>
       <c r="I12" s="19" t="s">
         <v>81</v>
@@ -12858,8 +12860,8 @@
       <c r="J12" s="3">
         <v>15</v>
       </c>
-      <c r="K12" s="684"/>
-      <c r="L12" s="699" t="s">
+      <c r="K12" s="677"/>
+      <c r="L12" s="692" t="s">
         <v>93</v>
       </c>
       <c r="M12" s="21" t="s">
@@ -12890,25 +12892,25 @@
         <v>116</v>
       </c>
       <c r="Y12" s="6"/>
-      <c r="AA12" s="688" t="s">
+      <c r="AA12" s="681" t="s">
         <v>126</v>
       </c>
-      <c r="AB12" s="689"/>
+      <c r="AB12" s="682"/>
       <c r="AC12" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="AD12" s="678"/>
+      <c r="AD12" s="671"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="702"/>
-      <c r="G13" s="666"/>
-      <c r="K13" s="684"/>
-      <c r="L13" s="700"/>
+      <c r="C13" s="663"/>
+      <c r="G13" s="698"/>
+      <c r="K13" s="677"/>
+      <c r="L13" s="693"/>
       <c r="M13" s="47"/>
-      <c r="Q13" s="668" t="s">
+      <c r="Q13" s="700" t="s">
         <v>210</v>
       </c>
-      <c r="R13" s="591"/>
+      <c r="R13" s="594"/>
       <c r="S13" s="525"/>
       <c r="T13" s="6"/>
       <c r="U13" s="96" t="s">
@@ -12917,17 +12919,17 @@
       <c r="X13" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="AA13" s="690"/>
-      <c r="AB13" s="691"/>
-      <c r="AD13" s="678"/>
+      <c r="AA13" s="683"/>
+      <c r="AB13" s="684"/>
+      <c r="AD13" s="671"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="C14" s="704"/>
+      <c r="C14" s="665"/>
       <c r="D14" s="23"/>
-      <c r="G14" s="666"/>
+      <c r="G14" s="698"/>
       <c r="H14" s="125"/>
       <c r="I14" s="99" t="s">
         <v>44</v>
@@ -12935,8 +12937,8 @@
       <c r="J14" s="111">
         <v>115</v>
       </c>
-      <c r="K14" s="684"/>
-      <c r="L14" s="700"/>
+      <c r="K14" s="677"/>
+      <c r="L14" s="693"/>
       <c r="M14" s="21" t="s">
         <v>111</v>
       </c>
@@ -12957,9 +12959,9 @@
       <c r="Y14" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="AA14" s="690"/>
-      <c r="AB14" s="691"/>
-      <c r="AD14" s="678"/>
+      <c r="AA14" s="683"/>
+      <c r="AB14" s="684"/>
+      <c r="AD14" s="671"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="130" t="s">
@@ -12974,19 +12976,19 @@
       <c r="F15" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="666"/>
+      <c r="G15" s="698"/>
       <c r="H15" s="2" t="s">
         <v>81</v>
       </c>
       <c r="I15" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="K15" s="684"/>
-      <c r="L15" s="701"/>
-      <c r="Q15" s="668" t="s">
+      <c r="K15" s="677"/>
+      <c r="L15" s="694"/>
+      <c r="Q15" s="700" t="s">
         <v>211</v>
       </c>
-      <c r="R15" s="591"/>
+      <c r="R15" s="594"/>
       <c r="S15" s="525"/>
       <c r="T15" s="6"/>
       <c r="V15" s="68" t="s">
@@ -12995,14 +12997,14 @@
       <c r="X15" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AA15" s="690"/>
-      <c r="AB15" s="691"/>
-      <c r="AD15" s="678"/>
+      <c r="AA15" s="683"/>
+      <c r="AB15" s="684"/>
+      <c r="AD15" s="671"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="132"/>
-      <c r="G16" s="666"/>
-      <c r="K16" s="684"/>
+      <c r="G16" s="698"/>
+      <c r="K16" s="677"/>
       <c r="N16" s="47"/>
       <c r="O16" s="61" t="s">
         <v>109</v>
@@ -13021,24 +13023,24 @@
       <c r="Z16" s="76" t="s">
         <v>127</v>
       </c>
-      <c r="AA16" s="690"/>
-      <c r="AB16" s="691"/>
-      <c r="AD16" s="678"/>
+      <c r="AA16" s="683"/>
+      <c r="AB16" s="684"/>
+      <c r="AD16" s="671"/>
     </row>
     <row r="17" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="109"/>
       <c r="E17" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F17" s="663" t="s">
+      <c r="F17" s="695" t="s">
         <v>96</v>
       </c>
-      <c r="G17" s="666"/>
+      <c r="G17" s="698"/>
       <c r="H17" s="54"/>
       <c r="I17" s="133" t="s">
         <v>81</v>
       </c>
-      <c r="K17" s="684"/>
+      <c r="K17" s="677"/>
       <c r="S17" s="525"/>
       <c r="V17" s="68" t="s">
         <v>44</v>
@@ -13046,9 +13048,9 @@
       <c r="X17" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="AA17" s="690"/>
-      <c r="AB17" s="691"/>
-      <c r="AD17" s="678"/>
+      <c r="AA17" s="683"/>
+      <c r="AB17" s="684"/>
+      <c r="AD17" s="671"/>
     </row>
     <row r="18" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="130"/>
@@ -13058,15 +13060,15 @@
       <c r="E18" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="664"/>
-      <c r="G18" s="666"/>
+      <c r="F18" s="696"/>
+      <c r="G18" s="698"/>
       <c r="H18" s="108" t="s">
         <v>76</v>
       </c>
       <c r="I18" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="K18" s="684"/>
+      <c r="K18" s="677"/>
       <c r="O18" s="64" t="s">
         <v>115</v>
       </c>
@@ -13077,39 +13079,42 @@
       <c r="X18" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="AA18" s="692"/>
-      <c r="AB18" s="693"/>
-      <c r="AD18" s="678"/>
+      <c r="AA18" s="685"/>
+      <c r="AB18" s="686"/>
+      <c r="AD18" s="671"/>
     </row>
     <row r="19" spans="3:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F19" s="64" t="s">
         <v>209</v>
       </c>
-      <c r="G19" s="667"/>
-      <c r="K19" s="685"/>
+      <c r="G19" s="699"/>
+      <c r="K19" s="678"/>
       <c r="Q19" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="R19" s="672" t="s">
+      <c r="R19" s="704" t="s">
         <v>124</v>
       </c>
-      <c r="S19" s="673"/>
-      <c r="T19" s="674"/>
+      <c r="S19" s="705"/>
+      <c r="T19" s="706"/>
       <c r="V19" s="77" t="s">
         <v>115</v>
       </c>
       <c r="Y19" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="AD19" s="679"/>
+      <c r="AD19" s="672"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="M10:AC10"/>
-    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G2:G19"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="L9:N9"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="S12:S18"/>
+    <mergeCell ref="O3:O9"/>
     <mergeCell ref="AD1:AD19"/>
     <mergeCell ref="S8:AC8"/>
     <mergeCell ref="K5:K19"/>
@@ -13121,14 +13126,11 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="L4:L8"/>
     <mergeCell ref="L12:L15"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G2:G19"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="S12:S18"/>
-    <mergeCell ref="O3:O9"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="M10:AC10"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ABC News Live ShieldW Halted
ABC News Live ShieldW Halted
</commit_message>
<xml_diff>
--- a/System_2.1.2.xlsx
+++ b/System_2.1.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E521CC-07D2-4C17-AEEB-9E9C6D433EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C327A0-78A1-4FFA-8A3C-06999DCAF2FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1781,9 +1781,6 @@
     <t>TBD</t>
   </si>
   <si>
-    <t>CBS</t>
-  </si>
-  <si>
     <t>X_Media_X</t>
   </si>
   <si>
@@ -1797,6 +1794,9 @@
   </si>
   <si>
     <t xml:space="preserve">Polimer </t>
+  </si>
+  <si>
+    <t>X - India - X</t>
   </si>
 </sst>
 </file>
@@ -3369,7 +3369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="710">
+  <cellXfs count="709">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -5165,7 +5165,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5458,7 +5457,7 @@
   <dimension ref="B1:U28"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5626,7 +5625,7 @@
         <v>228</v>
       </c>
       <c r="Q5" s="19">
-        <v>5040</v>
+        <v>5100</v>
       </c>
       <c r="S5" s="532"/>
     </row>
@@ -5678,7 +5677,7 @@
         <v>21</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="I7" s="61"/>
       <c r="J7" s="299"/>
@@ -5736,7 +5735,7 @@
         <v>21</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="I9" s="61"/>
       <c r="J9" s="297"/>
@@ -5766,7 +5765,7 @@
         <v>21</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="I10" s="61"/>
       <c r="J10" s="297"/>
@@ -5784,7 +5783,7 @@
         <v>227</v>
       </c>
       <c r="Q10" s="64">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="S10" s="532"/>
     </row>
@@ -5804,7 +5803,7 @@
         <v>21</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="I11" s="374"/>
       <c r="J11" s="295"/>
@@ -5867,7 +5866,7 @@
         <v>402</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="I13" s="61"/>
       <c r="J13" s="184"/>
@@ -5902,7 +5901,7 @@
         <v>21</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="I15" s="61"/>
       <c r="J15" s="136"/>
@@ -5938,7 +5937,7 @@
         <v>21</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="I16" s="61"/>
       <c r="J16" s="203"/>
@@ -6036,7 +6035,7 @@
         <v>391</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="I20" s="61"/>
       <c r="J20" s="167"/>
@@ -6066,7 +6065,7 @@
         <v>21</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="I21" s="61"/>
       <c r="J21" s="8"/>
@@ -6194,7 +6193,7 @@
         <v>21</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="I25" s="61"/>
       <c r="J25" s="139"/>
@@ -6314,8 +6313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB54FD83-008D-4F8B-87AC-83E7F70047CB}">
   <dimension ref="A1:W29"/>
   <sheetViews>
-    <sheetView topLeftCell="E11" workbookViewId="0">
-      <selection activeCell="U23" sqref="U23"/>
+    <sheetView topLeftCell="E10" workbookViewId="0">
+      <selection activeCell="W23" sqref="W23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6530,8 +6529,26 @@
       <c r="O7" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="P7" s="454" t="s">
+      <c r="P7" s="99" t="s">
+        <v>585</v>
+      </c>
+      <c r="Q7" s="127" t="s">
         <v>44</v>
+      </c>
+      <c r="R7" s="24">
+        <v>3</v>
+      </c>
+      <c r="S7" s="24">
+        <v>1</v>
+      </c>
+      <c r="U7" s="6" t="s">
+        <v>528</v>
+      </c>
+      <c r="V7" s="6">
+        <v>1</v>
+      </c>
+      <c r="W7" s="6" t="s">
+        <v>528</v>
       </c>
     </row>
     <row r="8" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6546,6 +6563,12 @@
       <c r="G8" s="525"/>
       <c r="I8" s="542"/>
       <c r="N8" s="80"/>
+      <c r="U8" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="V8" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="244" t="s">
@@ -6567,6 +6590,12 @@
         <v>550</v>
       </c>
       <c r="N9" s="80"/>
+      <c r="U9" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="V9" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="245" t="s">
@@ -6579,7 +6608,7 @@
       <c r="D10" s="108"/>
       <c r="E10" s="68">
         <f>Boat!S8</f>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G10" s="525"/>
       <c r="I10" s="542"/>
@@ -6622,18 +6651,21 @@
       <c r="N11" s="16" t="s">
         <v>424</v>
       </c>
-      <c r="P11" s="454" t="s">
+      <c r="P11" s="99" t="s">
+        <v>585</v>
+      </c>
+      <c r="Q11" s="127" t="s">
         <v>44</v>
       </c>
-      <c r="U11" s="6" t="s">
-        <v>479</v>
-      </c>
-      <c r="V11" s="6">
-        <v>1</v>
-      </c>
-      <c r="W11" s="6" t="s">
-        <v>479</v>
-      </c>
+      <c r="R11" s="24">
+        <v>0</v>
+      </c>
+      <c r="S11" s="24">
+        <v>2</v>
+      </c>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="6"/>
     </row>
     <row r="12" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="240" t="s">
@@ -6661,21 +6693,8 @@
       <c r="O12" s="68" t="s">
         <v>44</v>
       </c>
-      <c r="Q12" s="127" t="s">
-        <v>44</v>
-      </c>
-      <c r="R12" s="24">
-        <v>5</v>
-      </c>
-      <c r="S12" s="24">
-        <v>3</v>
-      </c>
-      <c r="U12" s="6" t="s">
-        <v>486</v>
-      </c>
-      <c r="V12" s="6">
-        <v>1</v>
-      </c>
+      <c r="U12" s="6"/>
+      <c r="V12" s="6"/>
       <c r="W12" s="6"/>
     </row>
     <row r="13" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6692,7 +6711,7 @@
       <c r="G13" s="525"/>
       <c r="I13" s="542"/>
       <c r="J13" s="108" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="K13" s="100" t="s">
         <v>44</v>
@@ -6706,19 +6725,13 @@
       <c r="N13" s="456" t="s">
         <v>547</v>
       </c>
-      <c r="U13" s="6" t="s">
-        <v>352</v>
-      </c>
-      <c r="V13" s="19">
-        <v>1</v>
-      </c>
-      <c r="W13" s="6" t="s">
-        <v>580</v>
-      </c>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6"/>
+      <c r="W13" s="6"/>
     </row>
     <row r="14" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="244" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B14" s="178" t="s">
         <v>150</v>
@@ -6738,15 +6751,6 @@
         <v>220</v>
       </c>
       <c r="I14" s="542"/>
-      <c r="Q14" s="127" t="s">
-        <v>44</v>
-      </c>
-      <c r="R14" s="24">
-        <v>0</v>
-      </c>
-      <c r="S14" s="24">
-        <v>2</v>
-      </c>
       <c r="U14" s="6"/>
       <c r="V14" s="6"/>
       <c r="W14" s="6"/>
@@ -6777,15 +6781,9 @@
       <c r="M15" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="U15" s="6" t="s">
-        <v>528</v>
-      </c>
-      <c r="V15" s="6">
-        <v>1</v>
-      </c>
-      <c r="W15" s="6" t="s">
-        <v>528</v>
-      </c>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
     </row>
     <row r="16" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C16" s="2" t="s">
@@ -6799,12 +6797,8 @@
         <v>44</v>
       </c>
       <c r="L16" s="6"/>
-      <c r="U16" s="6" t="s">
-        <v>466</v>
-      </c>
-      <c r="V16" s="6">
-        <v>1</v>
-      </c>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
     </row>
     <row r="17" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="244" t="s">
@@ -6832,12 +6826,8 @@
       <c r="M17" s="21" t="s">
         <v>441</v>
       </c>
-      <c r="U17" s="709" t="s">
-        <v>247</v>
-      </c>
-      <c r="V17" s="709">
-        <v>1</v>
-      </c>
+      <c r="U17" s="6"/>
+      <c r="V17" s="6"/>
     </row>
     <row r="18" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="244" t="s">
@@ -6859,17 +6849,40 @@
       <c r="I18" s="542"/>
       <c r="L18" s="16"/>
       <c r="M18" s="21"/>
-      <c r="U18" s="6"/>
-      <c r="V18" s="6"/>
-      <c r="W18" s="6"/>
+      <c r="O18" s="539" t="s">
+        <v>540</v>
+      </c>
+      <c r="P18" s="540"/>
+      <c r="Q18" s="127" t="s">
+        <v>44</v>
+      </c>
+      <c r="R18" s="24">
+        <v>3</v>
+      </c>
+      <c r="S18" s="24">
+        <v>1</v>
+      </c>
+      <c r="U18" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="V18" s="6">
+        <v>1</v>
+      </c>
+      <c r="W18" s="6" t="s">
+        <v>479</v>
+      </c>
     </row>
     <row r="19" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I19" s="542"/>
       <c r="M19" s="21" t="s">
         <v>443</v>
       </c>
-      <c r="U19" s="6"/>
-      <c r="V19" s="6"/>
+      <c r="U19" s="6" t="s">
+        <v>486</v>
+      </c>
+      <c r="V19" s="6">
+        <v>1</v>
+      </c>
       <c r="W19" s="6"/>
     </row>
     <row r="20" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6901,8 +6914,13 @@
       <c r="M20" s="21" t="s">
         <v>417</v>
       </c>
-      <c r="U20" s="6"/>
-      <c r="V20" s="6"/>
+      <c r="U20" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="V20" s="19">
+        <v>1</v>
+      </c>
+      <c r="W20" s="6"/>
     </row>
     <row r="21" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I21" s="542"/>
@@ -6933,7 +6951,7 @@
     </row>
     <row r="23" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D23" s="21" t="s">
         <v>417</v>
@@ -6942,10 +6960,6 @@
         <v>44</v>
       </c>
       <c r="I23" s="542"/>
-      <c r="O23" s="539" t="s">
-        <v>540</v>
-      </c>
-      <c r="P23" s="540"/>
       <c r="V23" s="6"/>
       <c r="W23" s="6"/>
     </row>
@@ -6955,10 +6969,10 @@
         <v>44</v>
       </c>
       <c r="R24" s="24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S24" s="24">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7100,7 +7114,7 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="O18:P18"/>
     <mergeCell ref="I2:I29"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="A6:A8"/>
@@ -7798,7 +7812,7 @@
       <c r="D10" s="142"/>
       <c r="E10" s="250">
         <f>Boat!S8</f>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F10" s="593"/>
       <c r="N10" s="475" t="s">
@@ -8543,7 +8557,7 @@
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="244" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B23" s="178" t="s">
         <v>367</v>
@@ -8859,8 +8873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AN37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P11" workbookViewId="0">
-      <selection activeCell="AL27" sqref="AL27"/>
+    <sheetView tabSelected="1" topLeftCell="Q10" workbookViewId="0">
+      <selection activeCell="AL17" sqref="AL17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8999,11 +9013,11 @@
       </c>
       <c r="K2" s="637">
         <f>SUM(K4:K29)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L2" s="639">
         <f>SUM(L4:L29)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M2" s="614">
         <f>SUM(K30:K37)* (-1)</f>
@@ -9105,7 +9119,7 @@
       </c>
       <c r="R3" s="159">
         <f>SUM(R4:R29)</f>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="S3" s="642"/>
       <c r="T3" s="560"/>
@@ -9119,7 +9133,7 @@
       </c>
       <c r="W3" s="187">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="X3" s="59">
         <f t="shared" si="0"/>
@@ -9127,15 +9141,15 @@
       </c>
       <c r="Y3" s="66">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="Z3" s="66">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AA3" s="66">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AB3" s="66">
         <f t="shared" ref="AB3:AK3" si="1">SUM(AB4:AB29)</f>
@@ -9143,7 +9157,7 @@
       </c>
       <c r="AC3" s="66">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AD3" s="66">
         <f t="shared" si="1"/>
@@ -9155,7 +9169,7 @@
       </c>
       <c r="AF3" s="66">
         <f>SUM(AF4:AF29)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AG3" s="412">
         <f t="shared" si="1"/>
@@ -9163,19 +9177,19 @@
       </c>
       <c r="AH3" s="100">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AI3" s="100">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AJ3" s="329">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AK3" s="330">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AN3" s="112"/>
     </row>
@@ -9592,7 +9606,7 @@
       </c>
       <c r="S8" s="340">
         <f>R3</f>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="T8" s="17"/>
       <c r="U8" s="348"/>
@@ -10184,11 +10198,11 @@
       </c>
       <c r="J15" s="363"/>
       <c r="K15" s="309">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15" s="311">
         <f t="shared" si="10"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M15" s="633"/>
       <c r="N15" s="20"/>
@@ -10200,7 +10214,7 @@
       </c>
       <c r="Q15" s="164"/>
       <c r="R15" s="157">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S15" s="338">
         <v>-2</v>
@@ -10210,48 +10224,46 @@
       <c r="V15" s="345"/>
       <c r="W15" s="190">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X15" s="314"/>
       <c r="Y15" s="117">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z15" s="308">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AA15" s="308">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AB15" s="308">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="AC15" s="312">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AD15" s="318"/>
       <c r="AE15" s="314"/>
       <c r="AF15" s="314">
         <f t="shared" si="6"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AG15" s="373"/>
-      <c r="AH15" s="158">
-        <v>1</v>
-      </c>
+      <c r="AH15" s="158"/>
       <c r="AI15" s="326">
         <f t="shared" si="7"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AJ15" s="327">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AK15" s="328">
         <f t="shared" si="9"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AL15" s="6" t="s">
         <v>232</v>
@@ -10600,7 +10612,7 @@
         <v>1</v>
       </c>
       <c r="AL19" s="16" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="AN19" s="112"/>
     </row>

</xml_diff>

<commit_message>
Violation Reported - Bug22 - 1 day Adjust
Violation Reported -
Vendors Included -
AajTak , Puthiyathalaimura (Media)
TCS(IT Vendor)

Operation Frizzed of these Service Providers , till resolution of the Issue
</commit_message>
<xml_diff>
--- a/System_2.1.2.xlsx
+++ b/System_2.1.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D93A156-9D00-4636-9662-8C6FF553E044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDA062B-5B18-4B84-8B71-CA9CD85335E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1019" uniqueCount="585">
   <si>
     <t>Zone</t>
   </si>
@@ -1703,9 +1703,6 @@
     <t>!M_25_NOC_X_EmployerLeft3_X_Halt_RJ</t>
   </si>
   <si>
-    <t xml:space="preserve">Parliament - </t>
-  </si>
-  <si>
     <t>Rw- Indore</t>
   </si>
   <si>
@@ -1791,6 +1788,12 @@
   </si>
   <si>
     <t>!M_15_NOC_X_Spouse_X_Drive_Media_X104X</t>
+  </si>
+  <si>
+    <t>Violation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCS </t>
   </si>
 </sst>
 </file>
@@ -3369,7 +3372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="705">
+  <cellXfs count="706">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -5156,6 +5159,9 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5669,7 +5675,7 @@
         <v>21</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="I7" s="61"/>
       <c r="J7" s="299"/>
@@ -5727,7 +5733,7 @@
         <v>21</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="I9" s="61"/>
       <c r="J9" s="297"/>
@@ -5757,7 +5763,7 @@
         <v>21</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="I10" s="61"/>
       <c r="J10" s="297"/>
@@ -5795,7 +5801,7 @@
         <v>21</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="I11" s="374"/>
       <c r="J11" s="295"/>
@@ -5849,7 +5855,7 @@
       </c>
       <c r="D13" s="61"/>
       <c r="E13" s="61" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="F13" s="281" t="s">
         <v>370</v>
@@ -5858,7 +5864,7 @@
         <v>402</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="I13" s="61"/>
       <c r="J13" s="184"/>
@@ -5887,13 +5893,13 @@
       <c r="D15" s="61"/>
       <c r="E15" s="66"/>
       <c r="F15" s="34" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="G15" s="136" t="s">
         <v>21</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="I15" s="61"/>
       <c r="J15" s="136"/>
@@ -5929,7 +5935,7 @@
         <v>21</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="I16" s="61"/>
       <c r="J16" s="203"/>
@@ -6027,7 +6033,7 @@
         <v>391</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="I20" s="61"/>
       <c r="J20" s="167"/>
@@ -6057,7 +6063,7 @@
         <v>21</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="I21" s="61"/>
       <c r="J21" s="8"/>
@@ -6185,7 +6191,7 @@
         <v>21</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="I25" s="61"/>
       <c r="J25" s="139"/>
@@ -6303,10 +6309,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB54FD83-008D-4F8B-87AC-83E7F70047CB}">
-  <dimension ref="A1:W29"/>
+  <dimension ref="A1:W30"/>
   <sheetViews>
-    <sheetView topLeftCell="E10" workbookViewId="0">
-      <selection activeCell="T22" sqref="T22"/>
+    <sheetView topLeftCell="E11" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6522,7 +6528,7 @@
         <v>103</v>
       </c>
       <c r="P7" s="99" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="Q7" s="127" t="s">
         <v>44</v>
@@ -6644,7 +6650,7 @@
         <v>424</v>
       </c>
       <c r="P11" s="99" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="Q11" s="127" t="s">
         <v>44</v>
@@ -6703,7 +6709,7 @@
       <c r="G13" s="521"/>
       <c r="I13" s="538"/>
       <c r="J13" s="108" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="K13" s="100" t="s">
         <v>44</v>
@@ -6723,7 +6729,7 @@
     </row>
     <row r="14" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="244" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B14" s="178" t="s">
         <v>150</v>
@@ -6822,21 +6828,6 @@
       <c r="V17" s="6"/>
     </row>
     <row r="18" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="244" t="s">
-        <v>583</v>
-      </c>
-      <c r="B18" s="21" t="s">
-        <v>564</v>
-      </c>
-      <c r="C18" s="491" t="s">
-        <v>155</v>
-      </c>
-      <c r="D18" s="435" t="s">
-        <v>538</v>
-      </c>
-      <c r="E18" s="490" t="s">
-        <v>44</v>
-      </c>
       <c r="G18" s="16"/>
       <c r="I18" s="538"/>
       <c r="L18" s="16"/>
@@ -6849,7 +6840,7 @@
         <v>44</v>
       </c>
       <c r="R18" s="24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S18" s="24">
         <v>0</v>
@@ -6870,14 +6861,12 @@
       <c r="U19" s="6" t="s">
         <v>486</v>
       </c>
-      <c r="V19" s="6">
-        <v>1</v>
-      </c>
+      <c r="V19" s="6"/>
       <c r="W19" s="6"/>
     </row>
     <row r="20" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="244" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B20" s="227" t="s">
         <v>530</v>
@@ -6886,7 +6875,7 @@
         <v>445</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="E20" s="428">
         <v>-1</v>
@@ -6907,9 +6896,7 @@
       <c r="U20" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="V20" s="19">
-        <v>1</v>
-      </c>
+      <c r="V20" s="19"/>
       <c r="W20" s="6"/>
     </row>
     <row r="21" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6929,7 +6916,7 @@
         <v>445</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="E22" s="382">
         <v>1</v>
@@ -6941,7 +6928,7 @@
     </row>
     <row r="23" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D23" s="21" t="s">
         <v>417</v>
@@ -6987,6 +6974,21 @@
       </c>
     </row>
     <row r="26" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="244" t="s">
+        <v>582</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>563</v>
+      </c>
+      <c r="C26" s="491" t="s">
+        <v>155</v>
+      </c>
+      <c r="D26" s="435" t="s">
+        <v>538</v>
+      </c>
+      <c r="E26" s="490" t="s">
+        <v>44</v>
+      </c>
       <c r="F26" s="16"/>
       <c r="G26" s="16"/>
       <c r="H26" s="6"/>
@@ -7005,7 +7007,7 @@
         <v>44</v>
       </c>
       <c r="R26" s="24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S26" s="24">
         <v>3</v>
@@ -7019,12 +7021,6 @@
       </c>
     </row>
     <row r="27" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="246" t="s">
-        <v>388</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>415</v>
-      </c>
       <c r="I27" s="538"/>
       <c r="O27" s="2" t="s">
         <v>99</v>
@@ -7035,6 +7031,12 @@
       <c r="R27" s="112"/>
       <c r="S27" s="112"/>
       <c r="U27" s="6"/>
+      <c r="V27">
+        <v>-1</v>
+      </c>
+      <c r="W27" s="19" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="28" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D28" s="176" t="s">
@@ -7047,11 +7049,11 @@
       <c r="Q28" s="6"/>
       <c r="R28" s="112"/>
       <c r="T28" s="39"/>
-      <c r="V28">
+      <c r="V28" s="6">
         <v>-1</v>
       </c>
       <c r="W28" s="19" t="s">
-        <v>95</v>
+        <v>235</v>
       </c>
     </row>
     <row r="29" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7072,11 +7074,13 @@
       <c r="R29" s="519"/>
       <c r="S29" s="112"/>
       <c r="T29" s="80"/>
-      <c r="V29" s="6">
-        <v>-1</v>
-      </c>
-      <c r="W29" s="6" t="s">
-        <v>235</v>
+    </row>
+    <row r="30" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="246" t="s">
+        <v>388</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>415</v>
       </c>
     </row>
   </sheetData>
@@ -7104,7 +7108,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8CFE6D2-5300-4D31-9A66-EC93F2A54B69}">
   <dimension ref="A1:AQ27"/>
   <sheetViews>
-    <sheetView topLeftCell="Q9" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="AJ26" sqref="AJ26"/>
     </sheetView>
   </sheetViews>
@@ -7206,7 +7210,7 @@
         <v>156</v>
       </c>
       <c r="Y1" s="601" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="Z1" s="458">
         <v>1</v>
@@ -8050,7 +8054,7 @@
       <c r="N14" s="6"/>
       <c r="O14" s="571"/>
       <c r="Q14" s="61" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="S14" s="169" t="s">
         <v>28</v>
@@ -8136,7 +8140,7 @@
     </row>
     <row r="16" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B16" s="21" t="s">
         <v>417</v>
@@ -8199,7 +8203,7 @@
       <c r="N17" s="6"/>
       <c r="O17" s="571"/>
       <c r="Q17" s="21" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="S17" s="169" t="s">
         <v>183</v>
@@ -8252,10 +8256,10 @@
     </row>
     <row r="18" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="517" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C18" s="506" t="s">
         <v>540</v>
@@ -8268,14 +8272,14 @@
       </c>
       <c r="F18" s="568"/>
       <c r="G18" s="374" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I18" s="20"/>
       <c r="J18" s="20"/>
       <c r="O18" s="571"/>
       <c r="Q18" s="112"/>
       <c r="R18" s="563" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="T18" s="100" t="s">
         <v>44</v>
@@ -8323,7 +8327,7 @@
       <c r="O19" s="571"/>
       <c r="R19" s="564"/>
       <c r="S19" s="30" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="U19" s="608"/>
       <c r="V19" s="146"/>
@@ -8357,7 +8361,7 @@
     </row>
     <row r="20" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="244" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B20" s="227" t="s">
         <v>530</v>
@@ -8366,7 +8370,7 @@
         <v>504</v>
       </c>
       <c r="D20" s="21" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="E20" s="489">
         <v>-1</v>
@@ -8422,10 +8426,10 @@
     </row>
     <row r="21" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="244" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C21" s="508" t="s">
         <v>504</v>
@@ -8462,7 +8466,7 @@
       </c>
       <c r="AE21" s="6"/>
       <c r="AF21" s="6" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="AG21" s="6"/>
       <c r="AH21" s="251" t="s">
@@ -8477,7 +8481,7 @@
       </c>
       <c r="AL21" s="6"/>
       <c r="AM21" s="480" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="AN21" s="587"/>
     </row>
@@ -8524,7 +8528,7 @@
     </row>
     <row r="23" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="244" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B23" s="178" t="s">
         <v>367</v>
@@ -8673,7 +8677,7 @@
         <v>504</v>
       </c>
       <c r="D26" s="61" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="E26" s="424">
         <v>1</v>
@@ -8688,7 +8692,7 @@
       </c>
       <c r="Q26" s="590"/>
       <c r="R26" s="565" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="T26" s="183"/>
       <c r="U26" s="471"/>
@@ -8733,14 +8737,14 @@
         <v>418</v>
       </c>
       <c r="D27" s="61" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="E27" s="281" t="s">
         <v>44</v>
       </c>
       <c r="F27" s="569"/>
       <c r="G27" s="61" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="O27" s="572"/>
       <c r="R27" s="566"/>
@@ -8754,7 +8758,7 @@
       <c r="V27" s="476"/>
       <c r="W27" s="149"/>
       <c r="X27" s="481" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="Y27" s="603"/>
       <c r="Z27" s="163"/>
@@ -8840,8 +8844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2029A93E-B53C-4201-9F17-439C144F3CF1}">
   <dimension ref="A1:AN37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J12" workbookViewId="0">
-      <selection activeCell="AF12" sqref="AF12"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AL7" sqref="AL7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9253,9 +9257,15 @@
         <f>IF((AI4-AJ4)&gt;AJ4,(AI4-AJ4),AJ4)</f>
         <v>0</v>
       </c>
-      <c r="AL4" s="6"/>
-      <c r="AM4" s="19"/>
-      <c r="AN4" s="112"/>
+      <c r="AL4" s="333" t="s">
+        <v>204</v>
+      </c>
+      <c r="AM4" s="19" t="s">
+        <v>583</v>
+      </c>
+      <c r="AN4" s="112" t="s">
+        <v>584</v>
+      </c>
     </row>
     <row r="5" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I5" s="430"/>
@@ -9512,12 +9522,8 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AL7" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="AM7" s="231" t="s">
-        <v>554</v>
-      </c>
+      <c r="AL7" s="6"/>
+      <c r="AM7" s="231"/>
       <c r="AN7" s="80"/>
     </row>
     <row r="8" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9703,9 +9709,7 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AL9" s="6" t="s">
-        <v>264</v>
-      </c>
+      <c r="AL9" s="6"/>
       <c r="AM9" s="19"/>
       <c r="AN9" s="112"/>
     </row>
@@ -9896,7 +9900,7 @@
         <v>1</v>
       </c>
       <c r="H12" s="61" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I12" s="430" t="s">
         <v>302</v>
@@ -10577,7 +10581,7 @@
         <v>1</v>
       </c>
       <c r="AL19" s="16" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="AN19" s="112"/>
     </row>
@@ -11076,7 +11080,9 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AA25" s="308"/>
+      <c r="AA25" s="308">
+        <v>0</v>
+      </c>
       <c r="AB25" s="308">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -11165,12 +11171,16 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AA26" s="308"/>
+      <c r="AA26" s="308">
+        <v>0</v>
+      </c>
       <c r="AB26" s="308">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AC26" s="312"/>
+      <c r="AC26" s="312">
+        <v>0</v>
+      </c>
       <c r="AD26" s="318"/>
       <c r="AE26" s="316"/>
       <c r="AF26" s="314">
@@ -11191,8 +11201,15 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AL26" s="6"/>
-      <c r="AN26" s="112"/>
+      <c r="AL26" s="705" t="s">
+        <v>256</v>
+      </c>
+      <c r="AM26" s="19" t="s">
+        <v>583</v>
+      </c>
+      <c r="AN26" s="112" t="s">
+        <v>584</v>
+      </c>
     </row>
     <row r="27" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E27" s="31" t="s">
@@ -12418,7 +12435,7 @@
   <dimension ref="A1:AE19"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12702,9 +12719,6 @@
       <c r="K6" s="673"/>
       <c r="L6" s="687"/>
       <c r="O6" s="704"/>
-      <c r="S6" s="104" t="s">
-        <v>20</v>
-      </c>
       <c r="T6" s="2" t="s">
         <v>101</v>
       </c>
@@ -12831,6 +12845,9 @@
         <v>44</v>
       </c>
       <c r="S11" s="70"/>
+      <c r="U11" s="104" t="s">
+        <v>20</v>
+      </c>
       <c r="Y11" s="68" t="s">
         <v>121</v>
       </c>

</xml_diff>